<commit_message>
Pictures and results of soa formation run
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>Alfa</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>100nm</t>
+  </si>
+  <si>
+    <t>SOA_formation_N_30000</t>
+  </si>
+  <si>
+    <t>30sect</t>
+  </si>
+  <si>
+    <t>run_20130619T183705</t>
+  </si>
+  <si>
+    <t>tuloste</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>jakauma katosi</t>
+  </si>
+  <si>
+    <t>Ongelmia jakauman kasvaessa</t>
+  </si>
+  <si>
+    <t>ylärajan ylitse</t>
   </si>
 </sst>
 </file>
@@ -473,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +572,9 @@
         <f>F3*0.00000000000000009*0.00000003*26908000000000000000*G3*0.000000001*26908000000000000000</f>
         <v>586472.77584000002</v>
       </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -885,7 +912,7 @@
         <v>1172945.55168</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -916,7 +943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -943,7 +970,7 @@
         <v>1759418.3275199998</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -974,7 +1001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1001,7 +1028,7 @@
         <v>146618.19396</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1029,7 +1056,7 @@
         <v>146618.19396</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>9</v>
       </c>
@@ -1053,7 +1080,7 @@
         <v>879709.16375999991</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>10</v>
       </c>
@@ -1078,9 +1105,17 @@
         <v>879709.16375999991</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -1091,8 +1126,8 @@
       <c r="D25" s="4">
         <v>30000</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>3</v>
+      <c r="E25" s="4">
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <v>0.3</v>
@@ -1101,11 +1136,20 @@
         <v>100</v>
       </c>
       <c r="H25" s="5">
-        <f>F25*0.0000000000000002*0.00000006*26908000000000000000*G25*0.000000001*26908000000000000000</f>
+        <f t="shared" ref="H25:H30" si="8">F25*0.0000000000000002*0.00000006*26908000000000000000*G25*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
       <c r="B26">
         <v>2</v>
       </c>
@@ -1115,8 +1159,8 @@
       <c r="D26">
         <v>30000</v>
       </c>
-      <c r="E26">
-        <v>0</v>
+      <c r="E26" t="s">
+        <v>3</v>
       </c>
       <c r="F26">
         <v>0.3</v>
@@ -1125,11 +1169,17 @@
         <v>100</v>
       </c>
       <c r="H26" s="2">
-        <f>F26*0.0000000000000002*0.00000006*26908000000000000000*G26*0.000000001*26908000000000000000</f>
+        <f t="shared" si="8"/>
         <v>260654567.04000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B27" s="4">
         <v>3</v>
       </c>
@@ -1139,8 +1189,8 @@
       <c r="D27" s="4">
         <v>30000</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>3</v>
+      <c r="E27" s="4">
+        <v>0</v>
       </c>
       <c r="F27" s="4">
         <v>0.6</v>
@@ -1149,11 +1199,17 @@
         <v>100</v>
       </c>
       <c r="H27" s="5">
-        <f>F27*0.0000000000000002*0.00000006*26908000000000000000*G27*0.000000001*26908000000000000000</f>
+        <f t="shared" si="8"/>
         <v>521309134.08000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B28">
         <v>4</v>
       </c>
@@ -1163,8 +1219,8 @@
       <c r="D28">
         <v>30000</v>
       </c>
-      <c r="E28">
-        <v>0</v>
+      <c r="E28" t="s">
+        <v>3</v>
       </c>
       <c r="F28">
         <v>0.6</v>
@@ -1173,11 +1229,14 @@
         <v>100</v>
       </c>
       <c r="H28" s="2">
-        <f>F28*0.0000000000000002*0.00000006*26908000000000000000*G28*0.000000001*26908000000000000000</f>
+        <f t="shared" si="8"/>
         <v>521309134.08000004</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="B29" s="4">
         <v>5</v>
       </c>
@@ -1187,8 +1246,8 @@
       <c r="D29" s="4">
         <v>30000</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>3</v>
+      <c r="E29" s="4">
+        <v>0</v>
       </c>
       <c r="F29" s="4">
         <v>0.9</v>
@@ -1197,11 +1256,17 @@
         <v>100</v>
       </c>
       <c r="H29" s="5">
-        <f>F29*0.0000000000000002*0.00000006*26908000000000000000*G29*0.000000001*26908000000000000000</f>
+        <f t="shared" si="8"/>
         <v>781963701.12</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B30">
         <v>6</v>
       </c>
@@ -1211,8 +1276,8 @@
       <c r="D30">
         <v>30000</v>
       </c>
-      <c r="E30">
-        <v>0</v>
+      <c r="E30" t="s">
+        <v>3</v>
       </c>
       <c r="F30">
         <v>0.9</v>
@@ -1221,8 +1286,14 @@
         <v>100</v>
       </c>
       <c r="H30" s="2">
-        <f>F30*0.0000000000000002*0.00000006*26908000000000000000*G30*0.000000001*26908000000000000000</f>
+        <f t="shared" si="8"/>
         <v>781963701.12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New runs and tools
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>Alfa</t>
   </si>
@@ -136,6 +136,39 @@
   </si>
   <si>
     <t>run_20130620T110239</t>
+  </si>
+  <si>
+    <t>temp_20130624T125953</t>
+  </si>
+  <si>
+    <t>10sect</t>
+  </si>
+  <si>
+    <t>SOA_formation_24062013_faster_10sect</t>
+  </si>
+  <si>
+    <t>1/(24*3600)</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>vap_wallsink</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>3nm 1#/cm3s klo 11-13</t>
+  </si>
+  <si>
+    <t>20day</t>
+  </si>
+  <si>
+    <t>1/9s</t>
+  </si>
+  <si>
+    <t>mass conserv error 560%</t>
   </si>
 </sst>
 </file>
@@ -256,7 +289,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,6 +300,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="4" fontId="5" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -571,17 +605,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" customWidth="1"/>
   </cols>
@@ -1387,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1420,7 +1455,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1453,7 +1488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1483,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -1513,7 +1548,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -1571,6 +1606,69 @@
       </c>
       <c r="J38" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I40" t="s">
+        <v>45</v>
+      </c>
+      <c r="J40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41">
+        <v>0.3</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" ref="H41" si="10">F41*0.0000000000000002*0.00000006*26908000000000000000*G41*0.000000001*26908000000000000000</f>
+        <v>260654567.04000002</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J41" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added runs, scripts and pictures
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
   <si>
     <t>Alfa</t>
   </si>
@@ -169,13 +169,97 @@
   </si>
   <si>
     <t>mass conserv error 560%</t>
+  </si>
+  <si>
+    <t>40sect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mass conserv error </t>
+  </si>
+  <si>
+    <t>SOA_formation_24062013_faster</t>
+  </si>
+  <si>
+    <t>temp_20130624T165623</t>
+  </si>
+  <si>
+    <t>temp_20130625T045024</t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013_test</t>
+  </si>
+  <si>
+    <t>1/9000s</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>1day</t>
+  </si>
+  <si>
+    <t>exponential</t>
+  </si>
+  <si>
+    <t>run_20130625T130812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3nm 1#/cm3s </t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013_test2</t>
+  </si>
+  <si>
+    <t>used chamber_runfile</t>
+  </si>
+  <si>
+    <t>used chamber_runfile2</t>
+  </si>
+  <si>
+    <t>EHDOTUS</t>
+  </si>
+  <si>
+    <t>run_20130625T134834</t>
+  </si>
+  <si>
+    <t>run_20130625T141155</t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013_test3</t>
+  </si>
+  <si>
+    <t>ei tullut mass conserv error</t>
+  </si>
+  <si>
+    <t>20sect</t>
+  </si>
+  <si>
+    <t>Ntot initial virheellinen</t>
+  </si>
+  <si>
+    <t>Ntot initial oikein</t>
+  </si>
+  <si>
+    <t>run_20130625T143638</t>
+  </si>
+  <si>
+    <t>run_20130625T145621</t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013_test4</t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013</t>
+  </si>
+  <si>
+    <t>80 ajoa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +300,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,13 +375,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -301,8 +394,11 @@
     <xf numFmtId="4" fontId="5" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,6 +1765,508 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I46" t="s">
+        <v>45</v>
+      </c>
+      <c r="J46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47">
+        <v>0.3</v>
+      </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" ref="H47" si="11">F47*0.0000000000000002*0.00000006*26908000000000000000*G47*0.000000001*26908000000000000000</f>
+        <v>260654567.04000002</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0.3</v>
+      </c>
+      <c r="G48">
+        <v>100</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" ref="H48" si="12">F48*0.0000000000000002*0.00000006*26908000000000000000*G48*0.000000001*26908000000000000000</f>
+        <v>260654567.04000002</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J48" t="s">
+        <v>47</v>
+      </c>
+      <c r="K48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0.3</v>
+      </c>
+      <c r="G51">
+        <v>0.25</v>
+      </c>
+      <c r="H51" s="2">
+        <f>F51*0.0000000000000002*0.00000006*26908000000000000000*G51*0.000000001*26908000000000000000</f>
+        <v>651636.41759999993</v>
+      </c>
+      <c r="I51" t="s">
+        <v>57</v>
+      </c>
+      <c r="J51" t="s">
+        <v>47</v>
+      </c>
+      <c r="K51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="12">
+        <v>1</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="12">
+        <v>0</v>
+      </c>
+      <c r="E55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>48</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0.3</v>
+      </c>
+      <c r="G58">
+        <v>0.25</v>
+      </c>
+      <c r="H58" s="2">
+        <f>F58*0.0000000000000002*0.00000006*26908000000000000000*G58*0.000000001*26908000000000000000</f>
+        <v>651636.41759999993</v>
+      </c>
+      <c r="I58" t="s">
+        <v>57</v>
+      </c>
+      <c r="J58" t="s">
+        <v>62</v>
+      </c>
+      <c r="K58" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="K59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" t="s">
+        <v>48</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0.3</v>
+      </c>
+      <c r="G62">
+        <v>0.25</v>
+      </c>
+      <c r="H62" s="2">
+        <f>F62*0.0000000000000002*0.00000006*26908000000000000000*G62*0.000000001*26908000000000000000</f>
+        <v>651636.41759999993</v>
+      </c>
+      <c r="I62" t="s">
+        <v>57</v>
+      </c>
+      <c r="J62" t="s">
+        <v>62</v>
+      </c>
+      <c r="K62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="K63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66">
+        <v>1000</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0.3</v>
+      </c>
+      <c r="G66">
+        <v>0.25</v>
+      </c>
+      <c r="H66" s="2">
+        <f>F66*0.0000000000000002*0.00000006*26908000000000000000*G66*0.000000001*26908000000000000000</f>
+        <v>651636.41759999993</v>
+      </c>
+      <c r="I66" t="s">
+        <v>57</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="K67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" t="s">
+        <v>48</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <v>1000</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0.3</v>
+      </c>
+      <c r="G70">
+        <v>0.25</v>
+      </c>
+      <c r="H70" s="2">
+        <f>F70*0.0000000000000002*0.00000006*26908000000000000000*G70*0.000000001*26908000000000000000</f>
+        <v>651636.41759999993</v>
+      </c>
+      <c r="I70" t="s">
+        <v>57</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="K71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I75" t="s">
+        <v>45</v>
+      </c>
+      <c r="J75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76">
+        <v>2000</v>
+      </c>
+      <c r="E76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76">
+        <v>0.3</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+      <c r="H76" s="2">
+        <f t="shared" ref="H76" si="13">F76*0.0000000000000002*0.00000006*26908000000000000000*G76*0.000000001*26908000000000000000</f>
+        <v>260654567.04000002</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results, pictures and renamed folder
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="104">
   <si>
     <t>Alfa</t>
   </si>
@@ -253,6 +253,81 @@
   </si>
   <si>
     <t>80 ajoa</t>
+  </si>
+  <si>
+    <t>SOA_formation_25062013_5sect</t>
+  </si>
+  <si>
+    <t>temp_20130625T165137</t>
+  </si>
+  <si>
+    <t>Yeild menee yli alfan</t>
+  </si>
+  <si>
+    <t>koska alussa Cvap ei ole nolla.</t>
+  </si>
+  <si>
+    <t>kannattaa katsoa kuva Y(t)</t>
+  </si>
+  <si>
+    <t>yeild pienenee kun deltaP kasvaa ja kaava ennustaa huonommin</t>
+  </si>
+  <si>
+    <t>gas_source</t>
+  </si>
+  <si>
+    <t>vap_wallsink_on</t>
+  </si>
+  <si>
+    <t>dilu_on</t>
+  </si>
+  <si>
+    <t>N, mu, sigma</t>
+  </si>
+  <si>
+    <t>2000, 10nm, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.4662e+05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.6065e+08</t>
+  </si>
+  <si>
+    <t>1/90s</t>
+  </si>
+  <si>
+    <t>1/900s</t>
+  </si>
+  <si>
+    <t>1/90000s</t>
+  </si>
+  <si>
+    <t>1/(5*24*3600)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>fail = no result</t>
+  </si>
+  <si>
+    <t>pictures</t>
+  </si>
+  <si>
+    <t>temp_20130625T190918</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>jne.</t>
+  </si>
+  <si>
+    <t>24 ajoa</t>
+  </si>
+  <si>
+    <t>SOA_formation_26062013</t>
   </si>
 </sst>
 </file>
@@ -313,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +408,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -375,14 +480,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -396,8 +506,19 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="10">
+    <cellStyle name="20% - Accent3" xfId="6" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="7" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="8" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="9" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
     <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -701,16 +822,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" customWidth="1"/>
@@ -2211,62 +2335,1101 @@
         <v>73</v>
       </c>
     </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>79</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="H74" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I74" t="s">
+        <v>45</v>
+      </c>
+      <c r="J74" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75">
+        <v>2000</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75">
+        <v>0.3</v>
+      </c>
+      <c r="G75">
+        <v>100</v>
+      </c>
+      <c r="H75" s="2">
+        <f t="shared" ref="H75" si="13">F75*0.0000000000000002*0.00000006*26908000000000000000*G75*0.000000001*26908000000000000000</f>
+        <v>260654567.04000002</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B79" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="13">
+        <v>1</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G80" s="13">
+        <v>1</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" s="13">
+        <v>1</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G81" s="14">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82">
+        <v>3</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" s="13">
+        <v>1</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G82" s="13">
+        <v>1</v>
+      </c>
+      <c r="I82" t="s">
+        <v>98</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E83" s="13">
+        <v>1</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G83" s="14">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E84" s="14">
+        <v>0</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G84" s="13">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>6</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" s="14">
+        <v>0</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G85" s="14">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>98</v>
+      </c>
+      <c r="L85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>7</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" s="14">
+        <v>0</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G86" s="13">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
+        <v>98</v>
+      </c>
+      <c r="L86" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" s="14">
+        <v>0</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E88" s="13">
+        <v>1</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G88" s="13">
+        <v>1</v>
+      </c>
+      <c r="I88" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E89" s="13">
+        <v>1</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G89" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>11</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E90" s="13">
+        <v>1</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G90" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>12</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E91" s="13">
+        <v>1</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>13</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" s="14">
+        <v>0</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G92" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>14</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E93" s="14">
+        <v>0</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G93" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>15</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E94" s="14">
+        <v>0</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G94" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>16</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E95" s="14">
+        <v>0</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G95" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>17</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E96" s="13">
+        <v>1</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G96" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>18</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E97" s="13">
+        <v>1</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G97" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>19</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E98" s="13">
+        <v>1</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G98" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>20</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E99" s="13">
+        <v>1</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G99" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>21</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E100" s="14">
+        <v>0</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G100" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>22</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E101" s="14">
+        <v>0</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G101" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>23</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E102" s="14">
+        <v>0</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G102" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>24</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E103" s="14">
+        <v>0</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G103" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>25</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E104" s="13">
+        <v>1</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G104" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>26</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E105" s="13">
+        <v>1</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G105" s="14">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>27</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E106" s="13">
+        <v>1</v>
+      </c>
+      <c r="F106" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G106" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>28</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" s="13">
+        <v>1</v>
+      </c>
+      <c r="F107" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G107" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>29</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E108" s="14">
+        <v>0</v>
+      </c>
+      <c r="F108" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G108" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>30</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E109" s="14">
+        <v>0</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G109" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>31</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E110" s="14">
+        <v>0</v>
+      </c>
+      <c r="F110" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G110" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>32</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E111" s="14">
+        <v>0</v>
+      </c>
+      <c r="F111" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G111" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>33</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E112" s="13">
+        <v>1</v>
+      </c>
+      <c r="F112" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G112" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>34</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D113" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E113" s="13">
+        <v>1</v>
+      </c>
+      <c r="F113" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G113" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>35</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D114" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E114" s="13">
+        <v>1</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G114" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>36</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D115" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E115" s="13">
+        <v>1</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G115" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>37</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D116" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E116" s="14">
+        <v>0</v>
+      </c>
+      <c r="F116" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G116" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>38</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D117" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E117" s="14">
+        <v>0</v>
+      </c>
+      <c r="F117" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G117" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>39</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D118" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E118" s="14">
+        <v>0</v>
+      </c>
+      <c r="F118" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G118" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>40</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D119" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E119" s="14">
+        <v>0</v>
+      </c>
+      <c r="F119" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G119" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>41</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D120" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E120" s="13">
+        <v>1</v>
+      </c>
+      <c r="F120" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G120" s="13">
+        <v>1</v>
+      </c>
+      <c r="I120" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>42</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E121" s="13">
+        <v>1</v>
+      </c>
+      <c r="F121" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G121" s="14">
+        <v>0</v>
+      </c>
+      <c r="I121" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>43</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E122" s="13">
+        <v>1</v>
+      </c>
+      <c r="F122" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G122" s="13">
+        <v>1</v>
+      </c>
+      <c r="I122" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I75" t="s">
+      <c r="D125" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>103</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D126" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J75" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" t="s">
-        <v>23</v>
-      </c>
-      <c r="D76">
-        <v>2000</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="E126" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F126" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G126" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H126" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I126" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D127" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E127" s="13">
+        <v>1</v>
+      </c>
+      <c r="F127" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F76">
-        <v>0.3</v>
-      </c>
-      <c r="G76">
-        <v>100</v>
-      </c>
-      <c r="H76" s="2">
-        <f t="shared" ref="H76" si="13">F76*0.0000000000000002*0.00000006*26908000000000000000*G76*0.000000001*26908000000000000000</f>
-        <v>260654567.04000002</v>
-      </c>
-      <c r="I76" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J76">
-        <v>0</v>
+      <c r="G127" s="13">
+        <v>1</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I127" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1day run results and pictures
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="138">
   <si>
     <t>Alfa</t>
   </si>
@@ -324,16 +324,121 @@
     <t>jne.</t>
   </si>
   <si>
-    <t>24 ajoa</t>
-  </si>
-  <si>
     <t>SOA_formation_26062013</t>
+  </si>
+  <si>
+    <t>run_20130627T071724</t>
+  </si>
+  <si>
+    <t>20 ajoa</t>
+  </si>
+  <si>
+    <t>Pariton fail = no results</t>
+  </si>
+  <si>
+    <t>Reason: dilu_coeff = 0;</t>
+  </si>
+  <si>
+    <t>All runs</t>
+  </si>
+  <si>
+    <t>mass conserv error 99%</t>
+  </si>
+  <si>
+    <t>Cvap(0) = 0;</t>
+  </si>
+  <si>
+    <t>SOA_formation_27062013_test</t>
+  </si>
+  <si>
+    <t>gas_source vector (daytime 11-13 gas_source on. Otherwise zero.</t>
+  </si>
+  <si>
+    <t>24 runs</t>
+  </si>
+  <si>
+    <t>SOA_formation_27062013</t>
+  </si>
+  <si>
+    <t>temp_20130627T122549</t>
+  </si>
+  <si>
+    <t>temp_20130627T124040</t>
+  </si>
+  <si>
+    <t>temp_20130627T151031</t>
+  </si>
+  <si>
+    <t>4000, 10nm, 1.3</t>
+  </si>
+  <si>
+    <t>fail no results</t>
+  </si>
+  <si>
+    <t>Yend ennustaa hyvin (täysin oikein)</t>
+  </si>
+  <si>
+    <t>Yend ennustaa kohdan jossa ollaan päästy maksimi Yeild</t>
+  </si>
+  <si>
+    <t>Paljonko prekursirista menee hiukkasiin tai seinille?</t>
+  </si>
+  <si>
+    <t>Hiukkasiin SOA (%)</t>
+  </si>
+  <si>
+    <t>Häviöt/seinä (%)</t>
+  </si>
+  <si>
+    <t>virhe kaavan ja mallin antaman tuloksen välillä</t>
+  </si>
+  <si>
+    <t>virhe kohdassa jossa ollaan päästy juuri maksimi yeild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuinka hyvin Yend kaava toimii? </t>
+  </si>
+  <si>
+    <t>Virhe verrattaessa kaavaa ja mallia.(%)</t>
+  </si>
+  <si>
+    <t>run_20130627T171225</t>
+  </si>
+  <si>
+    <t>SOA_formation_28062013_1day</t>
+  </si>
+  <si>
+    <t>run_20130628T122218</t>
+  </si>
+  <si>
+    <t>gas_source vector: 0.3*2e-16*60e-9*2.6908e19*100e-9*2.6908e19*exp(-2e-16.*60e-9.*2.6908e19.*tvect)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>HYVIÄ tuloksia !!!!!!!!!!!!!!!!!!!!!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>Virhe iso koska CS kasvaa hetkessä nopeasti isoon arvoon. Höyryä tulee nopeasti lisää.</t>
+  </si>
+  <si>
+    <t>Virhe verrattaessa kaavaa ja mallia. Kuinka paljon suurempi on Yend kuin Ymalli? (%)</t>
+  </si>
+  <si>
+    <t>P(0)</t>
+  </si>
+  <si>
+    <t>P = P(0)* exp(-kt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +493,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +545,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -480,7 +591,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -491,8 +602,9 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -512,8 +624,16 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="10"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
+    <cellStyle name="20% - Accent2" xfId="10" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="6" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="7" builtinId="42"/>
     <cellStyle name="20% - Accent5" xfId="8" builtinId="46"/>
@@ -822,23 +942,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N127"/>
+  <dimension ref="A1:N198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="B161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L184" sqref="L184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="50.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2465,6 +2589,9 @@
       <c r="I80" t="s">
         <v>98</v>
       </c>
+      <c r="J80" s="13" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
@@ -2496,7 +2623,7 @@
       <c r="A82" t="s">
         <v>100</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>3</v>
       </c>
       <c r="C82" s="13" t="s">
@@ -3154,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>34</v>
       </c>
@@ -3174,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>35</v>
       </c>
@@ -3194,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>36</v>
       </c>
@@ -3214,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>37</v>
       </c>
@@ -3234,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>38</v>
       </c>
@@ -3254,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>39</v>
       </c>
@@ -3274,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>40</v>
       </c>
@@ -3294,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>41</v>
       </c>
@@ -3317,7 +3444,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>42</v>
       </c>
@@ -3340,7 +3467,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>43</v>
       </c>
@@ -3363,7 +3490,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -3374,12 +3501,12 @@
         <v>48</v>
       </c>
       <c r="D125" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>103</v>
       </c>
       <c r="B126" s="12" t="s">
         <v>4</v>
@@ -3406,9 +3533,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>1</v>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>90</v>
@@ -3419,8 +3549,8 @@
       <c r="E127" s="13">
         <v>1</v>
       </c>
-      <c r="F127" s="13" t="s">
-        <v>43</v>
+      <c r="F127" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="G127" s="13">
         <v>1</v>
@@ -3428,8 +3558,1741 @@
       <c r="H127" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I127" t="s">
+      <c r="J127" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>4</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G128">
+        <v>1</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>6</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>8</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>10</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D131" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>12</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D132" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="J132" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>14</v>
+      </c>
+      <c r="C133" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>16</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>18</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>20</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D136" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>110</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B140" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F140" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G140" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H140" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I140" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B141" s="5">
+        <v>1</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D141" s="13">
+        <v>0</v>
+      </c>
+      <c r="E141" s="13">
+        <v>1</v>
+      </c>
+      <c r="F141" s="19">
+        <v>0</v>
+      </c>
+      <c r="G141" s="13">
+        <v>1</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I141" t="s">
         <v>98</v>
+      </c>
+      <c r="J141" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D142" s="13">
+        <v>0</v>
+      </c>
+      <c r="E142" s="13">
+        <v>1</v>
+      </c>
+      <c r="F142" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G142" s="13">
+        <v>1</v>
+      </c>
+      <c r="I142" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>116</v>
+      </c>
+      <c r="B143" s="5">
+        <v>3</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D143" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E143" s="13">
+        <v>1</v>
+      </c>
+      <c r="F143" s="19">
+        <v>0</v>
+      </c>
+      <c r="G143" s="13">
+        <v>1</v>
+      </c>
+      <c r="I143" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>113</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F146" t="s">
+        <v>111</v>
+      </c>
+      <c r="L146" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>128</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E147" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F147" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G147" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H147" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I147" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J147" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="K147" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L147" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="M147" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B148" s="5">
+        <v>1</v>
+      </c>
+      <c r="C148" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D148" s="13">
+        <v>0</v>
+      </c>
+      <c r="E148" s="13">
+        <v>1</v>
+      </c>
+      <c r="F148" s="19">
+        <v>0</v>
+      </c>
+      <c r="G148" s="13">
+        <v>1</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I148" t="s">
+        <v>98</v>
+      </c>
+      <c r="J148" t="s">
+        <v>119</v>
+      </c>
+      <c r="K148">
+        <v>0</v>
+      </c>
+      <c r="L148">
+        <v>100</v>
+      </c>
+      <c r="M148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>2</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D149" s="13">
+        <v>0</v>
+      </c>
+      <c r="E149" s="13">
+        <v>1</v>
+      </c>
+      <c r="F149" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G149" s="13">
+        <v>1</v>
+      </c>
+      <c r="I149" t="s">
+        <v>98</v>
+      </c>
+      <c r="J149" t="s">
+        <v>119</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>100</v>
+      </c>
+      <c r="M149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B150" s="5">
+        <v>3</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D150" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E150" s="13">
+        <v>1</v>
+      </c>
+      <c r="F150" s="19">
+        <v>0</v>
+      </c>
+      <c r="G150" s="13">
+        <v>1</v>
+      </c>
+      <c r="I150" t="s">
+        <v>98</v>
+      </c>
+      <c r="J150" t="s">
+        <v>120</v>
+      </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M150">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>4</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D151" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E151" s="13">
+        <v>1</v>
+      </c>
+      <c r="F151" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G151" s="13">
+        <v>1</v>
+      </c>
+      <c r="I151" t="s">
+        <v>98</v>
+      </c>
+      <c r="J151" t="s">
+        <v>120</v>
+      </c>
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M151">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B152" s="5">
+        <v>5</v>
+      </c>
+      <c r="C152" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E152" s="13">
+        <v>1</v>
+      </c>
+      <c r="F152" s="19">
+        <v>0</v>
+      </c>
+      <c r="G152" s="13">
+        <v>1</v>
+      </c>
+      <c r="I152" t="s">
+        <v>98</v>
+      </c>
+      <c r="J152" t="s">
+        <v>125</v>
+      </c>
+      <c r="K152">
+        <v>7.4</v>
+      </c>
+      <c r="L152">
+        <v>0.84</v>
+      </c>
+      <c r="M152">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>6</v>
+      </c>
+      <c r="C153" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D153" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E153" s="13">
+        <v>1</v>
+      </c>
+      <c r="F153" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G153" s="13">
+        <v>1</v>
+      </c>
+      <c r="I153" t="s">
+        <v>98</v>
+      </c>
+      <c r="J153" t="s">
+        <v>124</v>
+      </c>
+      <c r="K153">
+        <v>6.4</v>
+      </c>
+      <c r="L153">
+        <v>0.76</v>
+      </c>
+      <c r="M153">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B154" s="5">
+        <v>7</v>
+      </c>
+      <c r="C154" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D154" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E154" s="13">
+        <v>1</v>
+      </c>
+      <c r="F154" s="19">
+        <v>0</v>
+      </c>
+      <c r="G154" s="13">
+        <v>1</v>
+      </c>
+      <c r="I154" t="s">
+        <v>98</v>
+      </c>
+      <c r="K154">
+        <v>46</v>
+      </c>
+      <c r="L154" s="23">
+        <v>13.5</v>
+      </c>
+      <c r="M154">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>8</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D155" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E155" s="13">
+        <v>1</v>
+      </c>
+      <c r="F155" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G155" s="13">
+        <v>1</v>
+      </c>
+      <c r="I155" t="s">
+        <v>98</v>
+      </c>
+      <c r="J155" s="22"/>
+      <c r="K155">
+        <v>45.5</v>
+      </c>
+      <c r="L155">
+        <v>12.4</v>
+      </c>
+      <c r="M155">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B156" s="5">
+        <v>9</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D156" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E156" s="13">
+        <v>1</v>
+      </c>
+      <c r="F156" s="19">
+        <v>0</v>
+      </c>
+      <c r="G156" s="13">
+        <v>1</v>
+      </c>
+      <c r="I156" t="s">
+        <v>98</v>
+      </c>
+      <c r="K156">
+        <v>13</v>
+      </c>
+      <c r="L156">
+        <v>77.5</v>
+      </c>
+      <c r="M156">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>10</v>
+      </c>
+      <c r="C157" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E157" s="13">
+        <v>1</v>
+      </c>
+      <c r="F157" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G157" s="13">
+        <v>1</v>
+      </c>
+      <c r="I157" t="s">
+        <v>98</v>
+      </c>
+      <c r="K157">
+        <v>13.8</v>
+      </c>
+      <c r="L157">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="M157">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B158" s="5">
+        <v>11</v>
+      </c>
+      <c r="C158" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D158" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E158" s="13">
+        <v>1</v>
+      </c>
+      <c r="F158" s="19">
+        <v>0</v>
+      </c>
+      <c r="G158" s="13">
+        <v>1</v>
+      </c>
+      <c r="I158" t="s">
+        <v>98</v>
+      </c>
+      <c r="K158">
+        <v>1.4</v>
+      </c>
+      <c r="L158">
+        <v>97.4</v>
+      </c>
+      <c r="M158">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>12</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D159" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E159" s="13">
+        <v>1</v>
+      </c>
+      <c r="F159" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G159" s="13">
+        <v>1</v>
+      </c>
+      <c r="I159" t="s">
+        <v>98</v>
+      </c>
+      <c r="K159">
+        <v>1.9</v>
+      </c>
+      <c r="L159">
+        <v>96.9</v>
+      </c>
+      <c r="M159">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B160" s="5">
+        <v>13</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D160" s="13">
+        <v>0</v>
+      </c>
+      <c r="E160" s="13">
+        <v>1</v>
+      </c>
+      <c r="F160" s="19">
+        <v>0</v>
+      </c>
+      <c r="G160" s="13">
+        <v>1</v>
+      </c>
+      <c r="I160" t="s">
+        <v>98</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>100</v>
+      </c>
+      <c r="M160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>14</v>
+      </c>
+      <c r="C161" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D161" s="13">
+        <v>0</v>
+      </c>
+      <c r="E161" s="13">
+        <v>1</v>
+      </c>
+      <c r="F161" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G161" s="13">
+        <v>1</v>
+      </c>
+      <c r="I161" t="s">
+        <v>98</v>
+      </c>
+      <c r="K161">
+        <v>0</v>
+      </c>
+      <c r="L161">
+        <v>99.99</v>
+      </c>
+      <c r="M161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B162" s="5">
+        <v>15</v>
+      </c>
+      <c r="C162" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D162" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E162" s="13">
+        <v>1</v>
+      </c>
+      <c r="F162" s="19">
+        <v>0</v>
+      </c>
+      <c r="G162" s="13">
+        <v>1</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J162" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="K162" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L162" t="s">
+        <v>132</v>
+      </c>
+      <c r="M162" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>16</v>
+      </c>
+      <c r="C163" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D163" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E163" s="13">
+        <v>1</v>
+      </c>
+      <c r="F163" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G163" s="13">
+        <v>1</v>
+      </c>
+      <c r="I163" t="s">
+        <v>98</v>
+      </c>
+      <c r="J163" t="s">
+        <v>134</v>
+      </c>
+      <c r="K163">
+        <v>121</v>
+      </c>
+      <c r="L163">
+        <v>5</v>
+      </c>
+      <c r="M163">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B164" s="5">
+        <v>17</v>
+      </c>
+      <c r="C164" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D164" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E164" s="13">
+        <v>1</v>
+      </c>
+      <c r="F164" s="19">
+        <v>0</v>
+      </c>
+      <c r="G164" s="13">
+        <v>1</v>
+      </c>
+      <c r="I164" t="s">
+        <v>98</v>
+      </c>
+      <c r="K164">
+        <v>17.7</v>
+      </c>
+      <c r="L164">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="M164" s="25">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>18</v>
+      </c>
+      <c r="C165" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D165" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E165" s="13">
+        <v>1</v>
+      </c>
+      <c r="F165" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G165" s="13">
+        <v>1</v>
+      </c>
+      <c r="I165" t="s">
+        <v>98</v>
+      </c>
+      <c r="K165">
+        <v>18.2</v>
+      </c>
+      <c r="L165">
+        <v>70.3</v>
+      </c>
+      <c r="M165">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B166" s="5">
+        <v>19</v>
+      </c>
+      <c r="C166" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D166" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E166" s="13">
+        <v>1</v>
+      </c>
+      <c r="F166" s="19">
+        <v>0</v>
+      </c>
+      <c r="G166" s="13">
+        <v>1</v>
+      </c>
+      <c r="I166" t="s">
+        <v>98</v>
+      </c>
+      <c r="K166">
+        <v>1.8</v>
+      </c>
+      <c r="L166">
+        <v>96.7</v>
+      </c>
+      <c r="M166">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>20</v>
+      </c>
+      <c r="C167" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D167" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E167" s="13">
+        <v>1</v>
+      </c>
+      <c r="F167" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G167" s="13">
+        <v>1</v>
+      </c>
+      <c r="I167" t="s">
+        <v>98</v>
+      </c>
+      <c r="K167">
+        <v>1.76</v>
+      </c>
+      <c r="L167">
+        <v>96.6</v>
+      </c>
+      <c r="M167">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B168" s="5">
+        <v>21</v>
+      </c>
+      <c r="C168" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D168" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E168" s="13">
+        <v>1</v>
+      </c>
+      <c r="F168" s="19">
+        <v>0</v>
+      </c>
+      <c r="G168" s="13">
+        <v>1</v>
+      </c>
+      <c r="I168" t="s">
+        <v>98</v>
+      </c>
+      <c r="K168">
+        <v>-1.67</v>
+      </c>
+      <c r="L168">
+        <v>99.7</v>
+      </c>
+      <c r="M168">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>22</v>
+      </c>
+      <c r="C169" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D169" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E169" s="13">
+        <v>1</v>
+      </c>
+      <c r="F169" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G169" s="13">
+        <v>1</v>
+      </c>
+      <c r="I169" t="s">
+        <v>98</v>
+      </c>
+      <c r="K169">
+        <v>0.2</v>
+      </c>
+      <c r="L169">
+        <v>99.65</v>
+      </c>
+      <c r="M169">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B170" s="5">
+        <v>23</v>
+      </c>
+      <c r="C170" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D170" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E170" s="13">
+        <v>1</v>
+      </c>
+      <c r="F170" s="19">
+        <v>0</v>
+      </c>
+      <c r="G170" s="13">
+        <v>1</v>
+      </c>
+      <c r="I170" t="s">
+        <v>98</v>
+      </c>
+      <c r="K170">
+        <v>0.03</v>
+      </c>
+      <c r="L170">
+        <v>99.97</v>
+      </c>
+      <c r="M170">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>24</v>
+      </c>
+      <c r="C171" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D171" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E171" s="13">
+        <v>1</v>
+      </c>
+      <c r="F171" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G171" s="13">
+        <v>1</v>
+      </c>
+      <c r="I171" t="s">
+        <v>98</v>
+      </c>
+      <c r="K171">
+        <v>0</v>
+      </c>
+      <c r="L171">
+        <v>99.96</v>
+      </c>
+      <c r="M171">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>130</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F173" t="s">
+        <v>131</v>
+      </c>
+      <c r="L173" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>129</v>
+      </c>
+      <c r="B174" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D174" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E174" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F174" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G174" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H174" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I174" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J174" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="K174" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L174" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="M174" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B175" s="5">
+        <v>1</v>
+      </c>
+      <c r="C175" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D175" s="13">
+        <v>0</v>
+      </c>
+      <c r="E175" s="13">
+        <v>1</v>
+      </c>
+      <c r="F175" s="19">
+        <v>0</v>
+      </c>
+      <c r="G175" s="13">
+        <v>1</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>2</v>
+      </c>
+      <c r="C176" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D176" s="13">
+        <v>0</v>
+      </c>
+      <c r="E176" s="13">
+        <v>1</v>
+      </c>
+      <c r="F176" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G176" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B177" s="5">
+        <v>3</v>
+      </c>
+      <c r="C177" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D177" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E177" s="13">
+        <v>1</v>
+      </c>
+      <c r="F177" s="19">
+        <v>0</v>
+      </c>
+      <c r="G177" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D178" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E178" s="13">
+        <v>1</v>
+      </c>
+      <c r="F178" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G178" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B179" s="5">
+        <v>5</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D179" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E179" s="13">
+        <v>1</v>
+      </c>
+      <c r="F179" s="19">
+        <v>0</v>
+      </c>
+      <c r="G179" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>6</v>
+      </c>
+      <c r="C180" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D180" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E180" s="13">
+        <v>1</v>
+      </c>
+      <c r="F180" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G180" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B181" s="5">
+        <v>7</v>
+      </c>
+      <c r="C181" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D181" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E181" s="13">
+        <v>1</v>
+      </c>
+      <c r="F181" s="19">
+        <v>0</v>
+      </c>
+      <c r="G181" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>8</v>
+      </c>
+      <c r="C182" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D182" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E182" s="13">
+        <v>1</v>
+      </c>
+      <c r="F182" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G182" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="5">
+        <v>9</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D183" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E183" s="13">
+        <v>1</v>
+      </c>
+      <c r="F183" s="19">
+        <v>0</v>
+      </c>
+      <c r="G183" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>10</v>
+      </c>
+      <c r="C184" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D184" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E184" s="13">
+        <v>1</v>
+      </c>
+      <c r="F184" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G184" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B185" s="5">
+        <v>11</v>
+      </c>
+      <c r="C185" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D185" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E185" s="13">
+        <v>1</v>
+      </c>
+      <c r="F185" s="19">
+        <v>0</v>
+      </c>
+      <c r="G185" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>12</v>
+      </c>
+      <c r="C186" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D186" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E186" s="13">
+        <v>1</v>
+      </c>
+      <c r="F186" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G186" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B187" s="5">
+        <v>13</v>
+      </c>
+      <c r="C187" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D187" s="13">
+        <v>0</v>
+      </c>
+      <c r="E187" s="13">
+        <v>1</v>
+      </c>
+      <c r="F187" s="19">
+        <v>0</v>
+      </c>
+      <c r="G187" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>14</v>
+      </c>
+      <c r="C188" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D188" s="13">
+        <v>0</v>
+      </c>
+      <c r="E188" s="13">
+        <v>1</v>
+      </c>
+      <c r="F188" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G188" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B189" s="5">
+        <v>15</v>
+      </c>
+      <c r="C189" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E189" s="13">
+        <v>1</v>
+      </c>
+      <c r="F189" s="19">
+        <v>0</v>
+      </c>
+      <c r="G189" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>16</v>
+      </c>
+      <c r="C190" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D190" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E190" s="13">
+        <v>1</v>
+      </c>
+      <c r="F190" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G190" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B191" s="5">
+        <v>17</v>
+      </c>
+      <c r="C191" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D191" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E191" s="13">
+        <v>1</v>
+      </c>
+      <c r="F191" s="19">
+        <v>0</v>
+      </c>
+      <c r="G191" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>18</v>
+      </c>
+      <c r="C192" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D192" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E192" s="13">
+        <v>1</v>
+      </c>
+      <c r="F192" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G192" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B193" s="5">
+        <v>19</v>
+      </c>
+      <c r="C193" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D193" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E193" s="13">
+        <v>1</v>
+      </c>
+      <c r="F193" s="19">
+        <v>0</v>
+      </c>
+      <c r="G193" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>20</v>
+      </c>
+      <c r="C194" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D194" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E194" s="13">
+        <v>1</v>
+      </c>
+      <c r="F194" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G194" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B195" s="5">
+        <v>21</v>
+      </c>
+      <c r="C195" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D195" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E195" s="13">
+        <v>1</v>
+      </c>
+      <c r="F195" s="19">
+        <v>0</v>
+      </c>
+      <c r="G195" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>22</v>
+      </c>
+      <c r="C196" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D196" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E196" s="13">
+        <v>1</v>
+      </c>
+      <c r="F196" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G196" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B197" s="5">
+        <v>23</v>
+      </c>
+      <c r="C197" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D197" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E197" s="13">
+        <v>1</v>
+      </c>
+      <c r="F197" s="19">
+        <v>0</v>
+      </c>
+      <c r="G197" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>24</v>
+      </c>
+      <c r="C198" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D198" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E198" s="13">
+        <v>1</v>
+      </c>
+      <c r="F198" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G198" s="13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sripts, runs, results and pictures of those
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="193">
   <si>
     <t>Alfa</t>
   </si>
@@ -430,14 +430,181 @@
   </si>
   <si>
     <t>P = P(0)* exp(-kt)</t>
+  </si>
+  <si>
+    <t>SOA_formation_28062013_Ntot0_mp</t>
+  </si>
+  <si>
+    <t>SOA_formation_28062013_nucl_ps</t>
+  </si>
+  <si>
+    <t>Viikonlopuksi ajot</t>
+  </si>
+  <si>
+    <t>grew over maximum Dp</t>
+  </si>
+  <si>
+    <t>no results</t>
+  </si>
+  <si>
+    <t>run_20130629T053431</t>
+  </si>
+  <si>
+    <t>10day</t>
+  </si>
+  <si>
+    <t>ennustaa hyvin ensimmäisen päivän tilanteen mutta huononee kun aika kasvaa</t>
+  </si>
+  <si>
+    <t>0,5-15</t>
+  </si>
+  <si>
+    <t>0,85-70</t>
+  </si>
+  <si>
+    <t>Paulille annoin nukleaatiotilanteen ajettavaksi.</t>
+  </si>
+  <si>
+    <t>Ilmeisesti puolet epäonnistui.</t>
+  </si>
+  <si>
+    <t>Tulossa tuloksia ilmeisesti myöhemmin.</t>
+  </si>
+  <si>
+    <t>SOA_formation_01072013_uusiks_fail</t>
+  </si>
+  <si>
+    <t>epäonnistuneet runs 13-24</t>
+  </si>
+  <si>
+    <t>Uudestaan tilanteessa:</t>
+  </si>
+  <si>
+    <t>12 runs</t>
+  </si>
+  <si>
+    <t>run_20130701T210642</t>
+  </si>
+  <si>
+    <t>laskelmat tekemättä</t>
+  </si>
+  <si>
+    <t>Nämä tuloksen kunnolliseen tarkasteluun</t>
+  </si>
+  <si>
+    <t>Ei uusia tuloksia vaan vanhojen käsittelyä.</t>
+  </si>
+  <si>
+    <t>tau (days)</t>
+  </si>
+  <si>
+    <t>run_20130629T085050</t>
+  </si>
+  <si>
+    <t>Epäonnistuneet</t>
+  </si>
+  <si>
+    <t>indeksi</t>
+  </si>
+  <si>
+    <t>Virhe</t>
+  </si>
+  <si>
+    <t>wallsink</t>
+  </si>
+  <si>
+    <t>dilu</t>
+  </si>
+  <si>
+    <t>part_source</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Out of memory</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Event disappeared</t>
+  </si>
+  <si>
+    <t>Onnistuneet</t>
+  </si>
+  <si>
+    <t>aika</t>
+  </si>
+  <si>
+    <t>10days</t>
+  </si>
+  <si>
+    <t>Picture Yend(CSend)</t>
+  </si>
+  <si>
+    <t>Mark in matlab plot</t>
+  </si>
+  <si>
+    <t>o     circle</t>
+  </si>
+  <si>
+    <t>.     point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x     x-mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +     plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *     star</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> s     square</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> d     diamond</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v     triangle (down)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p     pentagram</t>
+  </si>
+  <si>
+    <t>h     hexagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ^     triangle (up)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;     triangle (left)</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>gas_source and part_source vector (daytime 11-13 gas_source on. Otherwise zero.</t>
+  </si>
+  <si>
+    <t>3nm nucl</t>
+  </si>
+  <si>
+    <t>1#/cm3s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -552,7 +719,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -590,6 +757,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -604,7 +851,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -631,6 +878,38 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent2" xfId="10" builtinId="34"/>
@@ -942,25 +1221,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N198"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L184" sqref="L184"/>
+    <sheetView tabSelected="1" topLeftCell="A279" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L298" sqref="L298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="50.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
@@ -4749,9 +5031,6 @@
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>130</v>
-      </c>
       <c r="B173" s="1" t="s">
         <v>51</v>
       </c>
@@ -4813,6 +5092,9 @@
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>130</v>
+      </c>
       <c r="B175" s="5">
         <v>1</v>
       </c>
@@ -4833,6 +5115,9 @@
       </c>
       <c r="H175" s="2" t="s">
         <v>117</v>
+      </c>
+      <c r="J175" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -4855,7 +5140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="5">
         <v>3</v>
       </c>
@@ -4875,7 +5160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>4</v>
       </c>
@@ -4895,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="5">
         <v>5</v>
       </c>
@@ -4914,8 +5199,11 @@
       <c r="G179" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>6</v>
       </c>
@@ -4934,8 +5222,11 @@
       <c r="G180" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B181" s="5">
         <v>7</v>
       </c>
@@ -4954,8 +5245,11 @@
       <c r="G181" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I181" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>8</v>
       </c>
@@ -4974,8 +5268,11 @@
       <c r="G182" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I182" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B183" s="5">
         <v>9</v>
       </c>
@@ -4995,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>10</v>
       </c>
@@ -5015,7 +5312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="5">
         <v>11</v>
       </c>
@@ -5035,7 +5332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>12</v>
       </c>
@@ -5055,7 +5352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B187" s="5">
         <v>13</v>
       </c>
@@ -5075,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>14</v>
       </c>
@@ -5095,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="5">
         <v>15</v>
       </c>
@@ -5115,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>16</v>
       </c>
@@ -5135,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B191" s="5">
         <v>17</v>
       </c>
@@ -5154,8 +5451,11 @@
       <c r="G191" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I191" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>18</v>
       </c>
@@ -5174,8 +5474,11 @@
       <c r="G192" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I192" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B193" s="5">
         <v>19</v>
       </c>
@@ -5194,8 +5497,11 @@
       <c r="G193" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I193" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>20</v>
       </c>
@@ -5214,8 +5520,11 @@
       <c r="G194" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I194" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B195" s="5">
         <v>21</v>
       </c>
@@ -5235,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>22</v>
       </c>
@@ -5255,7 +5564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B197" s="5">
         <v>23</v>
       </c>
@@ -5275,7 +5584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>24</v>
       </c>
@@ -5295,9 +5604,2395 @@
         <v>1</v>
       </c>
     </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F201" t="s">
+        <v>111</v>
+      </c>
+      <c r="L201" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>138</v>
+      </c>
+      <c r="B202" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C202" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D202" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E202" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F202" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G202" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H202" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I202" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J202" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="K202" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L202" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="M202" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>143</v>
+      </c>
+      <c r="B203" s="5">
+        <v>1</v>
+      </c>
+      <c r="C203" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D203" s="13">
+        <v>0</v>
+      </c>
+      <c r="E203" s="13">
+        <v>1</v>
+      </c>
+      <c r="F203" s="19">
+        <v>0</v>
+      </c>
+      <c r="G203" s="13">
+        <v>1</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I203" t="s">
+        <v>98</v>
+      </c>
+      <c r="K203">
+        <v>0.03</v>
+      </c>
+      <c r="L203">
+        <v>100</v>
+      </c>
+      <c r="M203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D204" s="13">
+        <v>0</v>
+      </c>
+      <c r="E204" s="13">
+        <v>1</v>
+      </c>
+      <c r="F204" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G204" s="13">
+        <v>1</v>
+      </c>
+      <c r="I204" t="s">
+        <v>98</v>
+      </c>
+      <c r="K204">
+        <v>0.5</v>
+      </c>
+      <c r="L204">
+        <v>99.7</v>
+      </c>
+      <c r="M204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B205" s="5">
+        <v>3</v>
+      </c>
+      <c r="C205" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D205" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E205" s="13">
+        <v>1</v>
+      </c>
+      <c r="F205" s="19">
+        <v>0</v>
+      </c>
+      <c r="G205" s="13">
+        <v>1</v>
+      </c>
+      <c r="I205" t="s">
+        <v>98</v>
+      </c>
+      <c r="J205" t="s">
+        <v>145</v>
+      </c>
+      <c r="K205" t="s">
+        <v>146</v>
+      </c>
+      <c r="L205">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M205">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>4</v>
+      </c>
+      <c r="C206" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D206" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E206" s="13">
+        <v>1</v>
+      </c>
+      <c r="F206" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G206" s="13">
+        <v>1</v>
+      </c>
+      <c r="I206" t="s">
+        <v>98</v>
+      </c>
+      <c r="J206" t="s">
+        <v>145</v>
+      </c>
+      <c r="K206" t="s">
+        <v>147</v>
+      </c>
+      <c r="L206">
+        <v>0.06</v>
+      </c>
+      <c r="M206">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B207" s="5">
+        <v>5</v>
+      </c>
+      <c r="C207" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D207" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E207" s="13">
+        <v>1</v>
+      </c>
+      <c r="F207" s="19">
+        <v>0</v>
+      </c>
+      <c r="G207" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>6</v>
+      </c>
+      <c r="C208" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D208" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E208" s="13">
+        <v>1</v>
+      </c>
+      <c r="F208" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G208" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B209" s="5">
+        <v>7</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D209" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E209" s="13">
+        <v>1</v>
+      </c>
+      <c r="F209" s="19">
+        <v>0</v>
+      </c>
+      <c r="G209" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>8</v>
+      </c>
+      <c r="C210" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D210" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E210" s="13">
+        <v>1</v>
+      </c>
+      <c r="F210" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G210" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B211" s="5">
+        <v>9</v>
+      </c>
+      <c r="C211" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D211" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E211" s="13">
+        <v>1</v>
+      </c>
+      <c r="F211" s="19">
+        <v>0</v>
+      </c>
+      <c r="G211" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>10</v>
+      </c>
+      <c r="C212" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D212" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E212" s="13">
+        <v>1</v>
+      </c>
+      <c r="F212" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G212" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B213" s="5">
+        <v>11</v>
+      </c>
+      <c r="C213" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D213" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E213" s="13">
+        <v>1</v>
+      </c>
+      <c r="F213" s="19">
+        <v>0</v>
+      </c>
+      <c r="G213" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>12</v>
+      </c>
+      <c r="C214" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D214" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E214" s="13">
+        <v>1</v>
+      </c>
+      <c r="F214" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G214" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B215" s="5">
+        <v>13</v>
+      </c>
+      <c r="C215" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D215" s="13">
+        <v>0</v>
+      </c>
+      <c r="E215" s="13">
+        <v>1</v>
+      </c>
+      <c r="F215" s="19">
+        <v>0</v>
+      </c>
+      <c r="G215" s="13">
+        <v>1</v>
+      </c>
+      <c r="I215" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>14</v>
+      </c>
+      <c r="C216" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D216" s="13">
+        <v>0</v>
+      </c>
+      <c r="E216" s="13">
+        <v>1</v>
+      </c>
+      <c r="F216" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G216" s="13">
+        <v>1</v>
+      </c>
+      <c r="I216" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B217" s="5">
+        <v>15</v>
+      </c>
+      <c r="C217" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D217" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E217" s="13">
+        <v>1</v>
+      </c>
+      <c r="F217" s="19">
+        <v>0</v>
+      </c>
+      <c r="G217" s="13">
+        <v>1</v>
+      </c>
+      <c r="I217" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>16</v>
+      </c>
+      <c r="C218" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D218" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E218" s="13">
+        <v>1</v>
+      </c>
+      <c r="F218" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G218" s="13">
+        <v>1</v>
+      </c>
+      <c r="I218" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B219" s="5">
+        <v>17</v>
+      </c>
+      <c r="C219" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D219" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E219" s="13">
+        <v>1</v>
+      </c>
+      <c r="F219" s="19">
+        <v>0</v>
+      </c>
+      <c r="G219" s="13">
+        <v>1</v>
+      </c>
+      <c r="I219" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>18</v>
+      </c>
+      <c r="C220" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D220" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E220" s="13">
+        <v>1</v>
+      </c>
+      <c r="F220" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G220" s="13">
+        <v>1</v>
+      </c>
+      <c r="I220" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B221" s="5">
+        <v>19</v>
+      </c>
+      <c r="C221" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D221" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E221" s="13">
+        <v>1</v>
+      </c>
+      <c r="F221" s="19">
+        <v>0</v>
+      </c>
+      <c r="G221" s="13">
+        <v>1</v>
+      </c>
+      <c r="I221" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>20</v>
+      </c>
+      <c r="C222" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D222" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E222" s="13">
+        <v>1</v>
+      </c>
+      <c r="F222" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G222" s="13">
+        <v>1</v>
+      </c>
+      <c r="I222" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B223" s="5">
+        <v>21</v>
+      </c>
+      <c r="C223" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D223" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E223" s="13">
+        <v>1</v>
+      </c>
+      <c r="F223" s="19">
+        <v>0</v>
+      </c>
+      <c r="G223" s="13">
+        <v>1</v>
+      </c>
+      <c r="I223" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>22</v>
+      </c>
+      <c r="C224" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D224" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E224" s="13">
+        <v>1</v>
+      </c>
+      <c r="F224" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G224" s="13">
+        <v>1</v>
+      </c>
+      <c r="I224" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B225" s="5">
+        <v>23</v>
+      </c>
+      <c r="C225" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D225" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E225" s="13">
+        <v>1</v>
+      </c>
+      <c r="F225" s="19">
+        <v>0</v>
+      </c>
+      <c r="G225" s="13">
+        <v>1</v>
+      </c>
+      <c r="I225" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>24</v>
+      </c>
+      <c r="C226" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D226" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E226" s="13">
+        <v>1</v>
+      </c>
+      <c r="F226" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G226" s="13">
+        <v>1</v>
+      </c>
+      <c r="I226" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C229" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C230" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C231" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>160</v>
+      </c>
+      <c r="H232"/>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B233" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H233"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>161</v>
+      </c>
+      <c r="D234" t="s">
+        <v>162</v>
+      </c>
+      <c r="E234" t="s">
+        <v>163</v>
+      </c>
+      <c r="F234" t="s">
+        <v>164</v>
+      </c>
+      <c r="G234" t="s">
+        <v>165</v>
+      </c>
+      <c r="H234" t="s">
+        <v>166</v>
+      </c>
+      <c r="I234" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D235">
+        <v>1</v>
+      </c>
+      <c r="E235" t="s">
+        <v>167</v>
+      </c>
+      <c r="F235">
+        <v>0</v>
+      </c>
+      <c r="G235">
+        <v>0</v>
+      </c>
+      <c r="H235">
+        <v>1</v>
+      </c>
+      <c r="I235" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D236">
+        <v>11</v>
+      </c>
+      <c r="E236" t="s">
+        <v>168</v>
+      </c>
+      <c r="F236" s="46">
+        <v>1.11E-5</v>
+      </c>
+      <c r="G236">
+        <v>0</v>
+      </c>
+      <c r="H236">
+        <v>1</v>
+      </c>
+      <c r="I236" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D237">
+        <v>13</v>
+      </c>
+      <c r="E237" t="s">
+        <v>167</v>
+      </c>
+      <c r="F237">
+        <v>0</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
+      <c r="H237">
+        <v>1</v>
+      </c>
+      <c r="I237" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D238">
+        <v>14</v>
+      </c>
+      <c r="E238" t="s">
+        <v>169</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+      <c r="G238" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H238">
+        <v>1</v>
+      </c>
+      <c r="I238" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D239">
+        <v>15</v>
+      </c>
+      <c r="E239" t="s">
+        <v>167</v>
+      </c>
+      <c r="F239">
+        <v>0.1111</v>
+      </c>
+      <c r="G239">
+        <v>0</v>
+      </c>
+      <c r="H239">
+        <v>1</v>
+      </c>
+      <c r="I239" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D240">
+        <v>16</v>
+      </c>
+      <c r="E240" t="s">
+        <v>167</v>
+      </c>
+      <c r="F240">
+        <v>0.1111</v>
+      </c>
+      <c r="G240" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H240">
+        <v>1</v>
+      </c>
+      <c r="I240" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="241" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D241">
+        <v>19</v>
+      </c>
+      <c r="E241" t="s">
+        <v>167</v>
+      </c>
+      <c r="F241">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G241">
+        <v>0</v>
+      </c>
+      <c r="H241">
+        <v>1</v>
+      </c>
+      <c r="I241" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="242" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D242">
+        <v>20</v>
+      </c>
+      <c r="E242" t="s">
+        <v>170</v>
+      </c>
+      <c r="F242">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G242" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H242">
+        <v>1</v>
+      </c>
+      <c r="I242" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="243" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D243">
+        <v>21</v>
+      </c>
+      <c r="E243" t="s">
+        <v>167</v>
+      </c>
+      <c r="F243" s="46">
+        <v>1.111E-4</v>
+      </c>
+      <c r="G243">
+        <v>0</v>
+      </c>
+      <c r="H243">
+        <v>1</v>
+      </c>
+      <c r="I243" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="244" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D244">
+        <v>22</v>
+      </c>
+      <c r="E244" t="s">
+        <v>167</v>
+      </c>
+      <c r="F244" s="46">
+        <v>1.111E-4</v>
+      </c>
+      <c r="G244" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H244">
+        <v>1</v>
+      </c>
+      <c r="I244" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="245" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D245">
+        <v>23</v>
+      </c>
+      <c r="E245" t="s">
+        <v>167</v>
+      </c>
+      <c r="F245" s="46">
+        <v>1.111E-5</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="246" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D246">
+        <v>24</v>
+      </c>
+      <c r="E246" t="s">
+        <v>167</v>
+      </c>
+      <c r="F246" s="46">
+        <v>1.11E-5</v>
+      </c>
+      <c r="G246" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H246">
+        <v>1</v>
+      </c>
+      <c r="I246" s="46">
+        <v>260650000</v>
+      </c>
+    </row>
+    <row r="247" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H247"/>
+    </row>
+    <row r="248" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H248"/>
+    </row>
+    <row r="249" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>171</v>
+      </c>
+      <c r="D249" t="s">
+        <v>162</v>
+      </c>
+      <c r="E249" t="s">
+        <v>172</v>
+      </c>
+      <c r="F249" t="s">
+        <v>164</v>
+      </c>
+      <c r="G249" t="s">
+        <v>165</v>
+      </c>
+      <c r="H249" t="s">
+        <v>166</v>
+      </c>
+      <c r="I249" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="250" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>2</v>
+      </c>
+      <c r="F250" s="47">
+        <v>0</v>
+      </c>
+      <c r="G250" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H250">
+        <v>1</v>
+      </c>
+      <c r="I250" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="251" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D251">
+        <v>3</v>
+      </c>
+      <c r="F251" s="48">
+        <v>0.111</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
+      </c>
+      <c r="H251">
+        <v>1</v>
+      </c>
+      <c r="I251" s="46">
+        <v>147000</v>
+      </c>
+    </row>
+    <row r="252" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D252">
+        <v>4</v>
+      </c>
+      <c r="F252" s="48">
+        <v>0.111</v>
+      </c>
+      <c r="G252" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H252">
+        <v>1</v>
+      </c>
+      <c r="I252" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="253" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D253">
+        <v>5</v>
+      </c>
+      <c r="F253" s="48">
+        <v>1.11E-2</v>
+      </c>
+      <c r="G253">
+        <v>0</v>
+      </c>
+      <c r="H253">
+        <v>1</v>
+      </c>
+      <c r="I253" s="46">
+        <v>146620</v>
+      </c>
+      <c r="J253" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="254" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D254">
+        <v>6</v>
+      </c>
+      <c r="F254" s="48">
+        <v>1.11E-2</v>
+      </c>
+      <c r="G254" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H254">
+        <v>1</v>
+      </c>
+      <c r="I254" s="46">
+        <v>146620</v>
+      </c>
+      <c r="J254" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="255" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D255">
+        <v>7</v>
+      </c>
+      <c r="F255" s="48">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255">
+        <v>1</v>
+      </c>
+      <c r="I255" s="46">
+        <v>146620</v>
+      </c>
+      <c r="J255" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="256" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D256">
+        <v>8</v>
+      </c>
+      <c r="F256" s="48">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G256" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H256">
+        <v>1</v>
+      </c>
+      <c r="I256" s="46">
+        <v>146620</v>
+      </c>
+      <c r="J256" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D257">
+        <v>9</v>
+      </c>
+      <c r="F257" s="48">
+        <v>1.111E-4</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+      <c r="H257">
+        <v>1</v>
+      </c>
+      <c r="I257" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D258">
+        <v>10</v>
+      </c>
+      <c r="F258" s="48">
+        <v>1.111E-4</v>
+      </c>
+      <c r="G258" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H258">
+        <v>1</v>
+      </c>
+      <c r="I258" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D259">
+        <v>12</v>
+      </c>
+      <c r="F259" s="48">
+        <v>1.111E-5</v>
+      </c>
+      <c r="G259" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H259">
+        <v>1</v>
+      </c>
+      <c r="I259" s="46">
+        <v>146620</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D260">
+        <v>17</v>
+      </c>
+      <c r="F260" s="48">
+        <v>1.11E-2</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>1</v>
+      </c>
+      <c r="I260" s="46">
+        <v>260650000</v>
+      </c>
+      <c r="J260" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D261">
+        <v>18</v>
+      </c>
+      <c r="F261" s="48">
+        <v>1.11E-2</v>
+      </c>
+      <c r="G261" s="46">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="H261">
+        <v>1</v>
+      </c>
+      <c r="I261" s="46">
+        <v>260650000</v>
+      </c>
+      <c r="J261" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>138</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F266" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>152</v>
+      </c>
+      <c r="B267" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C267" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D267" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E267" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F267" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G267" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H267" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I267" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>155</v>
+      </c>
+      <c r="B268" s="5">
+        <v>1</v>
+      </c>
+      <c r="C268" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D268" s="13">
+        <v>0</v>
+      </c>
+      <c r="E268" s="13">
+        <v>1</v>
+      </c>
+      <c r="F268" s="19">
+        <v>0</v>
+      </c>
+      <c r="G268" s="13">
+        <v>1</v>
+      </c>
+      <c r="H268" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>2</v>
+      </c>
+      <c r="C269" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D269" s="13">
+        <v>0</v>
+      </c>
+      <c r="E269" s="13">
+        <v>1</v>
+      </c>
+      <c r="F269" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G269" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B270" s="5">
+        <v>3</v>
+      </c>
+      <c r="C270" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D270" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E270" s="13">
+        <v>1</v>
+      </c>
+      <c r="F270" s="19">
+        <v>0</v>
+      </c>
+      <c r="G270" s="13">
+        <v>1</v>
+      </c>
+      <c r="I270" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <v>4</v>
+      </c>
+      <c r="C271" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D271" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E271" s="13">
+        <v>1</v>
+      </c>
+      <c r="F271" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G271" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B272" s="5">
+        <v>5</v>
+      </c>
+      <c r="C272" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D272" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E272" s="13">
+        <v>1</v>
+      </c>
+      <c r="F272" s="19">
+        <v>0</v>
+      </c>
+      <c r="G272" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>6</v>
+      </c>
+      <c r="C273" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D273" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E273" s="13">
+        <v>1</v>
+      </c>
+      <c r="F273" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G273" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B274" s="5">
+        <v>7</v>
+      </c>
+      <c r="C274" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D274" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E274" s="13">
+        <v>1</v>
+      </c>
+      <c r="F274" s="19">
+        <v>0</v>
+      </c>
+      <c r="G274" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>8</v>
+      </c>
+      <c r="C275" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D275" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E275" s="13">
+        <v>1</v>
+      </c>
+      <c r="F275" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G275" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B276" s="5">
+        <v>9</v>
+      </c>
+      <c r="C276" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D276" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E276" s="13">
+        <v>1</v>
+      </c>
+      <c r="F276" s="19">
+        <v>0</v>
+      </c>
+      <c r="G276" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>10</v>
+      </c>
+      <c r="C277" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D277" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E277" s="13">
+        <v>1</v>
+      </c>
+      <c r="F277" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G277" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B278" s="5">
+        <v>11</v>
+      </c>
+      <c r="C278" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D278" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E278" s="13">
+        <v>1</v>
+      </c>
+      <c r="F278" s="19">
+        <v>0</v>
+      </c>
+      <c r="G278" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>12</v>
+      </c>
+      <c r="C279" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D279" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E279" s="13">
+        <v>1</v>
+      </c>
+      <c r="F279" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G279" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A283" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B283" s="26"/>
+      <c r="C283" s="26"/>
+      <c r="D283" s="26"/>
+      <c r="E283" s="26"/>
+      <c r="F283" s="26"/>
+      <c r="G283" s="26"/>
+      <c r="H283" s="27"/>
+      <c r="I283" s="26"/>
+      <c r="J283" s="26"/>
+      <c r="K283" s="28"/>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A284" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B284" s="30"/>
+      <c r="C284" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D284" s="30"/>
+      <c r="E284" s="30"/>
+      <c r="F284" s="30"/>
+      <c r="G284" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H284" s="38"/>
+      <c r="I284" s="32"/>
+      <c r="J284" s="32"/>
+      <c r="K284" s="33"/>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A285" s="29"/>
+      <c r="B285" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C285" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D285" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E285" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G285" s="32"/>
+      <c r="H285" s="38"/>
+      <c r="I285" s="32"/>
+      <c r="J285" s="32"/>
+      <c r="K285" s="33"/>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A286" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B286" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C286" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D286" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E286" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F286" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G286" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H286" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I286" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="J286" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="K286" s="57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A287" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B287" s="34">
+        <v>5</v>
+      </c>
+      <c r="C287" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D287" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E287" s="35">
+        <v>1</v>
+      </c>
+      <c r="F287" s="37">
+        <v>0</v>
+      </c>
+      <c r="G287" s="35">
+        <v>1</v>
+      </c>
+      <c r="H287" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="I287" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J287" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K287" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A288" s="29"/>
+      <c r="B288" s="32">
+        <v>6</v>
+      </c>
+      <c r="C288" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D288" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E288" s="35">
+        <v>1</v>
+      </c>
+      <c r="F288" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G288" s="35">
+        <v>1</v>
+      </c>
+      <c r="H288" s="38"/>
+      <c r="I288" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J288" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K288" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A289" s="29"/>
+      <c r="B289" s="34">
+        <v>7</v>
+      </c>
+      <c r="C289" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D289" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E289" s="35">
+        <v>1</v>
+      </c>
+      <c r="F289" s="37">
+        <v>0</v>
+      </c>
+      <c r="G289" s="35">
+        <v>1</v>
+      </c>
+      <c r="H289" s="38"/>
+      <c r="I289" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J289" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K289" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A290" s="29"/>
+      <c r="B290" s="32">
+        <v>8</v>
+      </c>
+      <c r="C290" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D290" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E290" s="35">
+        <v>1</v>
+      </c>
+      <c r="F290" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G290" s="35">
+        <v>1</v>
+      </c>
+      <c r="H290" s="38"/>
+      <c r="I290" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J290" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K290" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A291" s="29"/>
+      <c r="B291" s="34">
+        <v>17</v>
+      </c>
+      <c r="C291" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D291" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E291" s="35">
+        <v>1</v>
+      </c>
+      <c r="F291" s="37">
+        <v>0</v>
+      </c>
+      <c r="G291" s="35">
+        <v>1</v>
+      </c>
+      <c r="H291" s="38"/>
+      <c r="I291" s="32">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="J291" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K291" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A292" s="29"/>
+      <c r="B292" s="32">
+        <v>18</v>
+      </c>
+      <c r="C292" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D292" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E292" s="35">
+        <v>1</v>
+      </c>
+      <c r="F292" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G292" s="35">
+        <v>1</v>
+      </c>
+      <c r="H292" s="38"/>
+      <c r="I292" s="32">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="J292" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K292" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A293" s="29"/>
+      <c r="B293" s="34">
+        <v>19</v>
+      </c>
+      <c r="C293" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D293" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E293" s="35">
+        <v>1</v>
+      </c>
+      <c r="F293" s="37">
+        <v>0</v>
+      </c>
+      <c r="G293" s="35">
+        <v>1</v>
+      </c>
+      <c r="H293" s="38"/>
+      <c r="I293" s="32">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="J293" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K293" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A294" s="29"/>
+      <c r="B294" s="32">
+        <v>20</v>
+      </c>
+      <c r="C294" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D294" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E294" s="35">
+        <v>1</v>
+      </c>
+      <c r="F294" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G294" s="35">
+        <v>1</v>
+      </c>
+      <c r="H294" s="38"/>
+      <c r="I294" s="32">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="J294" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K294" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A295" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B295" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C295" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D295" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E295" s="32"/>
+      <c r="F295" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G295" s="32"/>
+      <c r="H295" s="38"/>
+      <c r="I295" s="32"/>
+      <c r="J295" s="32"/>
+      <c r="K295" s="33"/>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A296" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B296" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C296" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D296" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E296" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F296" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G296" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H296" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I296" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="J296" s="32"/>
+      <c r="K296" s="33"/>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A297" s="29"/>
+      <c r="B297" s="34">
+        <v>5</v>
+      </c>
+      <c r="C297" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D297" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E297" s="35">
+        <v>1</v>
+      </c>
+      <c r="F297" s="37">
+        <v>0</v>
+      </c>
+      <c r="G297" s="35">
+        <v>1</v>
+      </c>
+      <c r="H297" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="I297" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J297" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K297" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A298" s="29"/>
+      <c r="B298" s="32">
+        <v>6</v>
+      </c>
+      <c r="C298" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D298" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E298" s="35">
+        <v>1</v>
+      </c>
+      <c r="F298" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G298" s="35">
+        <v>1</v>
+      </c>
+      <c r="H298" s="38"/>
+      <c r="I298" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J298" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K298" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A299" s="29"/>
+      <c r="B299" s="34">
+        <v>7</v>
+      </c>
+      <c r="C299" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D299" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E299" s="35">
+        <v>1</v>
+      </c>
+      <c r="F299" s="37">
+        <v>0</v>
+      </c>
+      <c r="G299" s="35">
+        <v>1</v>
+      </c>
+      <c r="H299" s="38"/>
+      <c r="I299" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J299" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K299" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A300" s="29"/>
+      <c r="B300" s="32">
+        <v>8</v>
+      </c>
+      <c r="C300" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D300" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E300" s="35">
+        <v>1</v>
+      </c>
+      <c r="F300" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G300" s="35">
+        <v>1</v>
+      </c>
+      <c r="H300" s="38"/>
+      <c r="I300" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J300" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K300" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A301" s="29"/>
+      <c r="B301" s="34">
+        <v>17</v>
+      </c>
+      <c r="C301" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D301" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E301" s="35">
+        <v>1</v>
+      </c>
+      <c r="F301" s="37">
+        <v>0</v>
+      </c>
+      <c r="G301" s="35">
+        <v>1</v>
+      </c>
+      <c r="H301" s="38"/>
+      <c r="I301" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J301" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K301" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302" s="29"/>
+      <c r="B302" s="32">
+        <v>18</v>
+      </c>
+      <c r="C302" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D302" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E302" s="35">
+        <v>1</v>
+      </c>
+      <c r="F302" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G302" s="35">
+        <v>1</v>
+      </c>
+      <c r="H302" s="38"/>
+      <c r="I302" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J302" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K302" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A303" s="29"/>
+      <c r="B303" s="34">
+        <v>19</v>
+      </c>
+      <c r="C303" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D303" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E303" s="35">
+        <v>1</v>
+      </c>
+      <c r="F303" s="37">
+        <v>0</v>
+      </c>
+      <c r="G303" s="35">
+        <v>1</v>
+      </c>
+      <c r="H303" s="38"/>
+      <c r="I303" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J303" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K303" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A304" s="29"/>
+      <c r="B304" s="32">
+        <v>20</v>
+      </c>
+      <c r="C304" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D304" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E304" s="35">
+        <v>1</v>
+      </c>
+      <c r="F304" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G304" s="35">
+        <v>1</v>
+      </c>
+      <c r="H304" s="38"/>
+      <c r="I304" s="35">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J304" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K304" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A305" s="29"/>
+      <c r="B305" s="32"/>
+      <c r="C305" s="32"/>
+      <c r="D305" s="32"/>
+      <c r="E305" s="32"/>
+      <c r="F305" s="32"/>
+      <c r="G305" s="32"/>
+      <c r="H305" s="38"/>
+      <c r="I305" s="32"/>
+      <c r="J305" s="32"/>
+      <c r="K305" s="33"/>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A306" s="29"/>
+      <c r="B306" s="32"/>
+      <c r="C306" s="32"/>
+      <c r="D306" s="32"/>
+      <c r="E306" s="32"/>
+      <c r="F306" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="G306" s="32"/>
+      <c r="H306" s="38"/>
+      <c r="I306" s="32"/>
+      <c r="J306" s="32"/>
+      <c r="K306" s="33"/>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A307" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B307" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C307" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D307" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E307" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F307" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="G307" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H307" s="38"/>
+      <c r="I307" s="32"/>
+      <c r="J307" s="32"/>
+      <c r="K307" s="33"/>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A308" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B308" s="32">
+        <v>5</v>
+      </c>
+      <c r="C308" s="32"/>
+      <c r="D308" s="49">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E308" s="32">
+        <v>0</v>
+      </c>
+      <c r="F308" s="32">
+        <v>1</v>
+      </c>
+      <c r="G308" s="50">
+        <v>146620</v>
+      </c>
+      <c r="H308" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="I308" s="51">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J308" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="K308" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A309" s="29"/>
+      <c r="B309" s="32">
+        <v>6</v>
+      </c>
+      <c r="C309" s="32"/>
+      <c r="D309" s="49">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E309" s="50">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="F309" s="32">
+        <v>1</v>
+      </c>
+      <c r="G309" s="50">
+        <v>146620</v>
+      </c>
+      <c r="H309" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="I309" s="51">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J309" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="K309" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A310" s="29"/>
+      <c r="B310" s="32">
+        <v>7</v>
+      </c>
+      <c r="C310" s="32"/>
+      <c r="D310" s="49">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E310" s="32">
+        <v>0</v>
+      </c>
+      <c r="F310" s="32">
+        <v>1</v>
+      </c>
+      <c r="G310" s="50">
+        <v>146620</v>
+      </c>
+      <c r="H310" s="38"/>
+      <c r="I310" s="51">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J310" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="K310" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A311" s="29"/>
+      <c r="B311" s="32">
+        <v>8</v>
+      </c>
+      <c r="C311" s="32"/>
+      <c r="D311" s="49">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E311" s="50">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="F311" s="32">
+        <v>1</v>
+      </c>
+      <c r="G311" s="50">
+        <v>146620</v>
+      </c>
+      <c r="H311" s="38"/>
+      <c r="I311" s="51">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J311" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="K311" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A312" s="29"/>
+      <c r="B312" s="32">
+        <v>17</v>
+      </c>
+      <c r="C312" s="32"/>
+      <c r="D312" s="49">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E312" s="32">
+        <v>0</v>
+      </c>
+      <c r="F312" s="32">
+        <v>1</v>
+      </c>
+      <c r="G312" s="50">
+        <v>260650000</v>
+      </c>
+      <c r="H312" s="38"/>
+      <c r="I312" s="51">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J312" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="K312" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A313" s="41"/>
+      <c r="B313" s="42">
+        <v>18</v>
+      </c>
+      <c r="C313" s="42"/>
+      <c r="D313" s="54">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E313" s="55">
+        <v>3.8580000000000002E-6</v>
+      </c>
+      <c r="F313" s="42">
+        <v>1</v>
+      </c>
+      <c r="G313" s="55">
+        <v>260650000</v>
+      </c>
+      <c r="H313" s="43"/>
+      <c r="I313" s="56">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="J313" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="K313" s="44" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D315" s="48"/>
+      <c r="G315" s="46"/>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D316" s="48"/>
+      <c r="E316" s="46"/>
+      <c r="G316" s="46"/>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D317" s="48"/>
+      <c r="E317" s="46"/>
+      <c r="G317" s="46"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Batch results and pictures
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="226">
   <si>
     <t>Alfa</t>
   </si>
@@ -595,6 +595,105 @@
   </si>
   <si>
     <t>1#/cm3s</t>
+  </si>
+  <si>
+    <t>SOA_formation_05072013_batch_10nm</t>
+  </si>
+  <si>
+    <t>P(0) ppb</t>
+  </si>
+  <si>
+    <t>0.3*2e-16*60e-9*2.6908e19*10e-9*2.6908e19*exp(-2e-16.*60e-9.*2.6908e19.*tvect)</t>
+  </si>
+  <si>
+    <t>Moa(0) µg/m3</t>
+  </si>
+  <si>
+    <t>vap_wallsink (1/s)</t>
+  </si>
+  <si>
+    <t>10hours</t>
+  </si>
+  <si>
+    <t>32runs</t>
+  </si>
+  <si>
+    <t>1/50s</t>
+  </si>
+  <si>
+    <t>1/500s</t>
+  </si>
+  <si>
+    <t>Dp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma </t>
+  </si>
+  <si>
+    <t>SOA_formation_05072013_batch_80nm</t>
+  </si>
+  <si>
+    <t>80nm</t>
+  </si>
+  <si>
+    <t>Csmax (days)</t>
+  </si>
+  <si>
+    <t>aik 0,13</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>kun tau = 0,2</t>
+  </si>
+  <si>
+    <t>niin Y ja Yend täsmäävät hyvin</t>
+  </si>
+  <si>
+    <t>eli silloin on sellainen CSend joka täsmää</t>
+  </si>
+  <si>
+    <t>kun tau = 0,18</t>
+  </si>
+  <si>
+    <t>EI KOVIN FYSIKAALISESTI</t>
+  </si>
+  <si>
+    <t>KAMMIOTA MALLINTAVA TILANNE</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt; 'ROSKIIN'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.0273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.0818</t>
+  </si>
+  <si>
+    <t>*1.0e+04</t>
+  </si>
+  <si>
+    <t>0.0311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.1557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.3114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0380</t>
+  </si>
+  <si>
+    <t>1.0e+05 *</t>
   </si>
 </sst>
 </file>
@@ -851,7 +950,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -910,6 +1009,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent2" xfId="10" builtinId="34"/>
@@ -1224,19 +1327,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N317"/>
+  <dimension ref="A1:N424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L298" sqref="L298"/>
+    <sheetView tabSelected="1" topLeftCell="B330" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K360" sqref="K360:L363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
@@ -7981,14 +8084,1785 @@
       <c r="G315" s="46"/>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D316" s="48"/>
-      <c r="E316" s="46"/>
-      <c r="G316" s="46"/>
+      <c r="A316" t="s">
+        <v>193</v>
+      </c>
+      <c r="B316" s="30"/>
+      <c r="C316" s="30"/>
+      <c r="D316" s="30"/>
+      <c r="E316" s="30"/>
+      <c r="F316" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G316" s="34"/>
+      <c r="H316" s="38"/>
+      <c r="I316" s="32"/>
+      <c r="J316" s="32"/>
+      <c r="K316" s="33"/>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D317" s="48"/>
-      <c r="E317" s="46"/>
-      <c r="G317" s="46"/>
+      <c r="B317" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E317" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F317" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="G317" s="32"/>
+      <c r="H317" s="38"/>
+      <c r="I317" s="32"/>
+      <c r="J317" s="32"/>
+      <c r="K317" s="33"/>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B318" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C318" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D318" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E318" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F318" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="G318" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="J318" s="30"/>
+      <c r="K318" s="57"/>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B319">
+        <v>1</v>
+      </c>
+      <c r="C319" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D319" s="13">
+        <v>10</v>
+      </c>
+      <c r="E319" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F319" s="13">
+        <v>8.2640000000000005E-2</v>
+      </c>
+      <c r="G319" s="13">
+        <v>0.1396</v>
+      </c>
+      <c r="J319" t="s">
+        <v>202</v>
+      </c>
+      <c r="K319" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B320">
+        <v>2</v>
+      </c>
+      <c r="C320" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D320" s="13">
+        <v>10</v>
+      </c>
+      <c r="E320" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F320">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G320" s="13">
+        <v>0.1396</v>
+      </c>
+      <c r="J320" t="s">
+        <v>165</v>
+      </c>
+      <c r="K320" s="46">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="321" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B321">
+        <v>3</v>
+      </c>
+      <c r="C321" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D321" s="14">
+        <v>50</v>
+      </c>
+      <c r="E321" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F321">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G321">
+        <v>0.2</v>
+      </c>
+      <c r="J321" t="s">
+        <v>203</v>
+      </c>
+      <c r="K321" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="322" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B322">
+        <v>4</v>
+      </c>
+      <c r="C322" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D322" s="14">
+        <v>50</v>
+      </c>
+      <c r="E322" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F322">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G322">
+        <v>0.11</v>
+      </c>
+      <c r="K322" s="2"/>
+    </row>
+    <row r="323" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B323">
+        <v>5</v>
+      </c>
+      <c r="C323" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D323" s="15">
+        <v>100</v>
+      </c>
+      <c r="E323" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F323">
+        <v>0.06</v>
+      </c>
+      <c r="G323">
+        <v>0.2</v>
+      </c>
+      <c r="H323" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J323" t="s">
+        <v>2</v>
+      </c>
+      <c r="K323" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="L323" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="324" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B324">
+        <v>6</v>
+      </c>
+      <c r="C324" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D324" s="15">
+        <v>100</v>
+      </c>
+      <c r="E324" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G324">
+        <v>0.13</v>
+      </c>
+      <c r="K324" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="L324" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="325" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B325">
+        <v>7</v>
+      </c>
+      <c r="C325" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D325" s="16">
+        <v>200</v>
+      </c>
+      <c r="E325" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K325" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="L325" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="326" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B326">
+        <v>8</v>
+      </c>
+      <c r="C326" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D326" s="16">
+        <v>200</v>
+      </c>
+      <c r="E326" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K326" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="L326" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="327" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B327">
+        <v>9</v>
+      </c>
+      <c r="C327" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D327" s="13">
+        <v>10</v>
+      </c>
+      <c r="E327" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="328" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B328">
+        <v>10</v>
+      </c>
+      <c r="C328" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D328" s="13">
+        <v>10</v>
+      </c>
+      <c r="E328" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="329" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B329">
+        <v>11</v>
+      </c>
+      <c r="C329" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D329" s="14">
+        <v>50</v>
+      </c>
+      <c r="E329" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="330" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B330">
+        <v>12</v>
+      </c>
+      <c r="C330" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D330" s="14">
+        <v>50</v>
+      </c>
+      <c r="E330" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F330" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="G330" s="14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="331" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B331">
+        <v>13</v>
+      </c>
+      <c r="C331" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D331" s="15">
+        <v>100</v>
+      </c>
+      <c r="E331" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="332" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B332">
+        <v>14</v>
+      </c>
+      <c r="C332" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D332" s="15">
+        <v>100</v>
+      </c>
+      <c r="E332" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H332" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="333" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B333">
+        <v>15</v>
+      </c>
+      <c r="C333" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D333" s="16">
+        <v>200</v>
+      </c>
+      <c r="E333" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="H333" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="334" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B334">
+        <v>16</v>
+      </c>
+      <c r="C334" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D334" s="16">
+        <v>200</v>
+      </c>
+      <c r="E334" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H334" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="335" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B335">
+        <v>17</v>
+      </c>
+      <c r="C335" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D335" s="13">
+        <v>10</v>
+      </c>
+      <c r="E335" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="336" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B336">
+        <v>18</v>
+      </c>
+      <c r="C336" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D336" s="13">
+        <v>10</v>
+      </c>
+      <c r="E336" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="337" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B337">
+        <v>19</v>
+      </c>
+      <c r="C337" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D337" s="14">
+        <v>50</v>
+      </c>
+      <c r="E337" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="338" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B338">
+        <v>20</v>
+      </c>
+      <c r="C338" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D338" s="14">
+        <v>50</v>
+      </c>
+      <c r="E338" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="339" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B339">
+        <v>21</v>
+      </c>
+      <c r="C339" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D339" s="15">
+        <v>100</v>
+      </c>
+      <c r="E339" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F339">
+        <v>0.06</v>
+      </c>
+      <c r="G339">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="340" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B340">
+        <v>22</v>
+      </c>
+      <c r="C340" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D340" s="15">
+        <v>100</v>
+      </c>
+      <c r="E340" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="341" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B341">
+        <v>23</v>
+      </c>
+      <c r="C341" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D341" s="16">
+        <v>200</v>
+      </c>
+      <c r="E341" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="342" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B342">
+        <v>24</v>
+      </c>
+      <c r="C342" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D342" s="16">
+        <v>200</v>
+      </c>
+      <c r="E342" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="343" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B343">
+        <v>25</v>
+      </c>
+      <c r="C343" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D343" s="13">
+        <v>10</v>
+      </c>
+      <c r="E343" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="344" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B344">
+        <v>26</v>
+      </c>
+      <c r="C344" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D344" s="13">
+        <v>10</v>
+      </c>
+      <c r="E344" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="345" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B345">
+        <v>27</v>
+      </c>
+      <c r="C345" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D345" s="14">
+        <v>50</v>
+      </c>
+      <c r="E345" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="346" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B346">
+        <v>28</v>
+      </c>
+      <c r="C346" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D346" s="14">
+        <v>50</v>
+      </c>
+      <c r="E346" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="347" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B347">
+        <v>29</v>
+      </c>
+      <c r="C347" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D347" s="15">
+        <v>100</v>
+      </c>
+      <c r="E347" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="348" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B348">
+        <v>30</v>
+      </c>
+      <c r="C348" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D348" s="15">
+        <v>100</v>
+      </c>
+      <c r="E348" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="349" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B349">
+        <v>31</v>
+      </c>
+      <c r="C349" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D349" s="16">
+        <v>200</v>
+      </c>
+      <c r="E349" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G349">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="350" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B350">
+        <v>32</v>
+      </c>
+      <c r="C350" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D350" s="16">
+        <v>200</v>
+      </c>
+      <c r="E350" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F350">
+        <v>0.06</v>
+      </c>
+      <c r="G350">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="351" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F351" t="s">
+        <v>208</v>
+      </c>
+      <c r="G351" s="1">
+        <v>0.13059999999999999</v>
+      </c>
+    </row>
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>204</v>
+      </c>
+      <c r="B353" s="30"/>
+      <c r="C353" s="30"/>
+      <c r="D353" s="30"/>
+      <c r="E353" s="30"/>
+      <c r="F353" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G353" s="34"/>
+      <c r="H353" s="38"/>
+    </row>
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B354" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E354" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F354" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="G354" s="32"/>
+      <c r="H354" s="38"/>
+    </row>
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>213</v>
+      </c>
+      <c r="B355" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C355" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D355" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E355" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F355" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="G355" s="45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>214</v>
+      </c>
+      <c r="B356">
+        <v>1</v>
+      </c>
+      <c r="C356" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D356" s="13">
+        <v>10</v>
+      </c>
+      <c r="E356" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F356" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="G356" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="J356" t="s">
+        <v>202</v>
+      </c>
+      <c r="K356" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>215</v>
+      </c>
+      <c r="B357">
+        <v>2</v>
+      </c>
+      <c r="C357" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D357" s="13">
+        <v>10</v>
+      </c>
+      <c r="E357" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G357">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J357" t="s">
+        <v>165</v>
+      </c>
+      <c r="K357" s="46">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B358">
+        <v>3</v>
+      </c>
+      <c r="C358" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D358" s="14">
+        <v>50</v>
+      </c>
+      <c r="E358" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="J358" t="s">
+        <v>203</v>
+      </c>
+      <c r="K358" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B359">
+        <v>4</v>
+      </c>
+      <c r="C359" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D359" s="14">
+        <v>50</v>
+      </c>
+      <c r="E359" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K359" s="2"/>
+    </row>
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B360">
+        <v>5</v>
+      </c>
+      <c r="C360" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D360" s="15">
+        <v>100</v>
+      </c>
+      <c r="E360" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="J360" t="s">
+        <v>2</v>
+      </c>
+      <c r="K360" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="L360" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B361">
+        <v>6</v>
+      </c>
+      <c r="C361" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D361" s="15">
+        <v>100</v>
+      </c>
+      <c r="E361" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K361" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="L361" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B362">
+        <v>7</v>
+      </c>
+      <c r="C362" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D362" s="16">
+        <v>200</v>
+      </c>
+      <c r="E362" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K362" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="L362" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B363">
+        <v>8</v>
+      </c>
+      <c r="C363" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D363" s="16">
+        <v>200</v>
+      </c>
+      <c r="E363" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K363" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="L363" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B364">
+        <v>9</v>
+      </c>
+      <c r="C364" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D364" s="13">
+        <v>10</v>
+      </c>
+      <c r="E364" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B365">
+        <v>10</v>
+      </c>
+      <c r="C365" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D365" s="13">
+        <v>10</v>
+      </c>
+      <c r="E365" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B366">
+        <v>11</v>
+      </c>
+      <c r="C366" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D366" s="14">
+        <v>50</v>
+      </c>
+      <c r="E366" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B367">
+        <v>12</v>
+      </c>
+      <c r="C367" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D367" s="14">
+        <v>50</v>
+      </c>
+      <c r="E367" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B368">
+        <v>13</v>
+      </c>
+      <c r="C368" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D368" s="15">
+        <v>100</v>
+      </c>
+      <c r="E368" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="369" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B369">
+        <v>14</v>
+      </c>
+      <c r="C369" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D369" s="15">
+        <v>100</v>
+      </c>
+      <c r="E369" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F369">
+        <v>0.06</v>
+      </c>
+      <c r="G369">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="370" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B370">
+        <v>15</v>
+      </c>
+      <c r="C370" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D370" s="16">
+        <v>200</v>
+      </c>
+      <c r="E370" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="371" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B371">
+        <v>16</v>
+      </c>
+      <c r="C371" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D371" s="16">
+        <v>200</v>
+      </c>
+      <c r="E371" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="372" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B372">
+        <v>17</v>
+      </c>
+      <c r="C372" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D372" s="13">
+        <v>10</v>
+      </c>
+      <c r="E372" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="373" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B373">
+        <v>18</v>
+      </c>
+      <c r="C373" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D373" s="13">
+        <v>10</v>
+      </c>
+      <c r="E373" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="374" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B374">
+        <v>19</v>
+      </c>
+      <c r="C374" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D374" s="14">
+        <v>50</v>
+      </c>
+      <c r="E374" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F374">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G374">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="375" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B375">
+        <v>20</v>
+      </c>
+      <c r="C375" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D375" s="14">
+        <v>50</v>
+      </c>
+      <c r="E375" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H375" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="376" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B376">
+        <v>21</v>
+      </c>
+      <c r="C376" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D376" s="15">
+        <v>100</v>
+      </c>
+      <c r="E376" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="H376" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="377" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B377">
+        <v>22</v>
+      </c>
+      <c r="C377" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D377" s="15">
+        <v>100</v>
+      </c>
+      <c r="E377" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H377" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="378" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B378">
+        <v>23</v>
+      </c>
+      <c r="C378" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D378" s="16">
+        <v>200</v>
+      </c>
+      <c r="E378" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="379" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B379">
+        <v>24</v>
+      </c>
+      <c r="C379" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D379" s="16">
+        <v>200</v>
+      </c>
+      <c r="E379" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="380" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B380">
+        <v>25</v>
+      </c>
+      <c r="C380" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D380" s="13">
+        <v>10</v>
+      </c>
+      <c r="E380" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="381" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B381">
+        <v>26</v>
+      </c>
+      <c r="C381" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D381" s="13">
+        <v>10</v>
+      </c>
+      <c r="E381" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="382" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B382">
+        <v>27</v>
+      </c>
+      <c r="C382" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D382" s="14">
+        <v>50</v>
+      </c>
+      <c r="E382" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="383" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B383">
+        <v>28</v>
+      </c>
+      <c r="C383" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D383" s="14">
+        <v>50</v>
+      </c>
+      <c r="E383" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="384" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B384">
+        <v>29</v>
+      </c>
+      <c r="C384" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D384" s="15">
+        <v>100</v>
+      </c>
+      <c r="E384" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G384">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B385">
+        <v>30</v>
+      </c>
+      <c r="C385" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D385" s="15">
+        <v>100</v>
+      </c>
+      <c r="E385" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B386">
+        <v>31</v>
+      </c>
+      <c r="C386" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D386" s="16">
+        <v>200</v>
+      </c>
+      <c r="E386" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B387">
+        <v>32</v>
+      </c>
+      <c r="C387" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D387" s="16">
+        <v>200</v>
+      </c>
+      <c r="E387" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F387">
+        <v>0.05</v>
+      </c>
+      <c r="G387">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F388" t="s">
+        <v>208</v>
+      </c>
+      <c r="G388">
+        <v>0.13059999999999999</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>204</v>
+      </c>
+      <c r="B390" s="30"/>
+      <c r="C390" s="30"/>
+      <c r="D390" s="30"/>
+      <c r="E390" s="30"/>
+      <c r="F390" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G390" s="34"/>
+      <c r="H390" s="38"/>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B391" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E391" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F391" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="G391" s="32"/>
+      <c r="H391" s="38"/>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B392" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C392" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D392" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E392" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F392" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="G392" s="45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B393">
+        <v>1</v>
+      </c>
+      <c r="C393" s="13">
+        <v>1</v>
+      </c>
+      <c r="D393" s="13">
+        <v>10</v>
+      </c>
+      <c r="E393" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F393" s="13"/>
+      <c r="G393" s="13"/>
+      <c r="J393" t="s">
+        <v>202</v>
+      </c>
+      <c r="K393" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B394">
+        <v>2</v>
+      </c>
+      <c r="C394" s="13">
+        <v>1</v>
+      </c>
+      <c r="D394" s="13">
+        <v>10</v>
+      </c>
+      <c r="E394" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="J394" t="s">
+        <v>165</v>
+      </c>
+      <c r="K394" s="46">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B395">
+        <v>3</v>
+      </c>
+      <c r="C395" s="13">
+        <v>1</v>
+      </c>
+      <c r="D395" s="14">
+        <v>50</v>
+      </c>
+      <c r="E395" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="J395" t="s">
+        <v>203</v>
+      </c>
+      <c r="K395" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B396">
+        <v>4</v>
+      </c>
+      <c r="C396" s="13">
+        <v>1</v>
+      </c>
+      <c r="D396" s="14">
+        <v>50</v>
+      </c>
+      <c r="E396" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K396" s="2"/>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B397">
+        <v>5</v>
+      </c>
+      <c r="C397" s="13">
+        <v>1</v>
+      </c>
+      <c r="D397" s="15">
+        <v>100</v>
+      </c>
+      <c r="E397" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="J397" t="s">
+        <v>2</v>
+      </c>
+      <c r="K397" t="s">
+        <v>216</v>
+      </c>
+      <c r="L397" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B398">
+        <v>6</v>
+      </c>
+      <c r="C398" s="13">
+        <v>1</v>
+      </c>
+      <c r="D398" s="15">
+        <v>100</v>
+      </c>
+      <c r="E398" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K398" t="s">
+        <v>217</v>
+      </c>
+      <c r="L398" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B399">
+        <v>7</v>
+      </c>
+      <c r="C399" s="13">
+        <v>1</v>
+      </c>
+      <c r="D399" s="16">
+        <v>200</v>
+      </c>
+      <c r="E399" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K399" t="s">
+        <v>218</v>
+      </c>
+      <c r="L399" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B400">
+        <v>8</v>
+      </c>
+      <c r="C400" s="13">
+        <v>1</v>
+      </c>
+      <c r="D400" s="16">
+        <v>200</v>
+      </c>
+      <c r="E400" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K400" t="s">
+        <v>219</v>
+      </c>
+      <c r="L400" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="401" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B401">
+        <v>9</v>
+      </c>
+      <c r="C401" s="14">
+        <v>5</v>
+      </c>
+      <c r="D401" s="13">
+        <v>10</v>
+      </c>
+      <c r="E401" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="402" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B402">
+        <v>10</v>
+      </c>
+      <c r="C402" s="14">
+        <v>5</v>
+      </c>
+      <c r="D402" s="13">
+        <v>10</v>
+      </c>
+      <c r="E402" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="403" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B403">
+        <v>11</v>
+      </c>
+      <c r="C403" s="14">
+        <v>5</v>
+      </c>
+      <c r="D403" s="14">
+        <v>50</v>
+      </c>
+      <c r="E403" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="404" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B404">
+        <v>12</v>
+      </c>
+      <c r="C404" s="14">
+        <v>5</v>
+      </c>
+      <c r="D404" s="14">
+        <v>50</v>
+      </c>
+      <c r="E404" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="405" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B405">
+        <v>13</v>
+      </c>
+      <c r="C405" s="14">
+        <v>5</v>
+      </c>
+      <c r="D405" s="15">
+        <v>100</v>
+      </c>
+      <c r="E405" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="406" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B406">
+        <v>14</v>
+      </c>
+      <c r="C406" s="14">
+        <v>5</v>
+      </c>
+      <c r="D406" s="15">
+        <v>100</v>
+      </c>
+      <c r="E406" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="407" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B407">
+        <v>15</v>
+      </c>
+      <c r="C407" s="14">
+        <v>5</v>
+      </c>
+      <c r="D407" s="16">
+        <v>200</v>
+      </c>
+      <c r="E407" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="408" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B408">
+        <v>16</v>
+      </c>
+      <c r="C408" s="14">
+        <v>5</v>
+      </c>
+      <c r="D408" s="16">
+        <v>200</v>
+      </c>
+      <c r="E408" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="409" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B409">
+        <v>17</v>
+      </c>
+      <c r="C409" s="15">
+        <v>10</v>
+      </c>
+      <c r="D409" s="13">
+        <v>10</v>
+      </c>
+      <c r="E409" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="410" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B410">
+        <v>18</v>
+      </c>
+      <c r="C410" s="15">
+        <v>10</v>
+      </c>
+      <c r="D410" s="13">
+        <v>10</v>
+      </c>
+      <c r="E410" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="411" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B411">
+        <v>19</v>
+      </c>
+      <c r="C411" s="15">
+        <v>10</v>
+      </c>
+      <c r="D411" s="14">
+        <v>50</v>
+      </c>
+      <c r="E411" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="412" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B412">
+        <v>20</v>
+      </c>
+      <c r="C412" s="15">
+        <v>10</v>
+      </c>
+      <c r="D412" s="14">
+        <v>50</v>
+      </c>
+      <c r="E412" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="413" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B413">
+        <v>21</v>
+      </c>
+      <c r="C413" s="15">
+        <v>10</v>
+      </c>
+      <c r="D413" s="15">
+        <v>100</v>
+      </c>
+      <c r="E413" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="414" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B414">
+        <v>22</v>
+      </c>
+      <c r="C414" s="15">
+        <v>10</v>
+      </c>
+      <c r="D414" s="15">
+        <v>100</v>
+      </c>
+      <c r="E414" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="415" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B415">
+        <v>23</v>
+      </c>
+      <c r="C415" s="15">
+        <v>10</v>
+      </c>
+      <c r="D415" s="16">
+        <v>200</v>
+      </c>
+      <c r="E415" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="416" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B416">
+        <v>24</v>
+      </c>
+      <c r="C416" s="15">
+        <v>10</v>
+      </c>
+      <c r="D416" s="16">
+        <v>200</v>
+      </c>
+      <c r="E416" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="417" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B417">
+        <v>25</v>
+      </c>
+      <c r="C417" s="16">
+        <v>30</v>
+      </c>
+      <c r="D417" s="13">
+        <v>10</v>
+      </c>
+      <c r="E417" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="418" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B418">
+        <v>26</v>
+      </c>
+      <c r="C418" s="16">
+        <v>30</v>
+      </c>
+      <c r="D418" s="13">
+        <v>10</v>
+      </c>
+      <c r="E418" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="419" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B419">
+        <v>27</v>
+      </c>
+      <c r="C419" s="16">
+        <v>30</v>
+      </c>
+      <c r="D419" s="14">
+        <v>50</v>
+      </c>
+      <c r="E419" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="420" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B420">
+        <v>28</v>
+      </c>
+      <c r="C420" s="16">
+        <v>30</v>
+      </c>
+      <c r="D420" s="14">
+        <v>50</v>
+      </c>
+      <c r="E420" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="421" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B421">
+        <v>29</v>
+      </c>
+      <c r="C421" s="16">
+        <v>30</v>
+      </c>
+      <c r="D421" s="15">
+        <v>100</v>
+      </c>
+      <c r="E421" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="422" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B422">
+        <v>30</v>
+      </c>
+      <c r="C422" s="16">
+        <v>30</v>
+      </c>
+      <c r="D422" s="15">
+        <v>100</v>
+      </c>
+      <c r="E422" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="423" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B423">
+        <v>31</v>
+      </c>
+      <c r="C423" s="16">
+        <v>30</v>
+      </c>
+      <c r="D423" s="16">
+        <v>200</v>
+      </c>
+      <c r="E423" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="424" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B424">
+        <v>32</v>
+      </c>
+      <c r="C424" s="16">
+        <v>30</v>
+      </c>
+      <c r="D424" s="16">
+        <v>200</v>
+      </c>
+      <c r="E424" s="14" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added and renamed batch pictures
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="232">
   <si>
     <t>Alfa</t>
   </si>
@@ -694,6 +694,24 @@
   </si>
   <si>
     <t>1.0e+05 *</t>
+  </si>
+  <si>
+    <t>kun tau = 0,08</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>SOA_formation_05072013_batch_80_isoMnm</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>magenta</t>
   </si>
 </sst>
 </file>
@@ -1327,10 +1345,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N424"/>
+  <dimension ref="A1:N425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B330" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K360" sqref="K360:L363"/>
+    <sheetView tabSelected="1" topLeftCell="A315" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H339" sqref="H339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7844,7 +7862,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A305" s="29"/>
       <c r="B305" s="32"/>
       <c r="C305" s="32"/>
@@ -7857,7 +7875,7 @@
       <c r="J305" s="32"/>
       <c r="K305" s="33"/>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306" s="29"/>
       <c r="B306" s="32"/>
       <c r="C306" s="32"/>
@@ -7872,7 +7890,7 @@
       <c r="J306" s="32"/>
       <c r="K306" s="33"/>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A307" s="53" t="s">
         <v>139</v>
       </c>
@@ -7899,7 +7917,7 @@
       <c r="J307" s="32"/>
       <c r="K307" s="33"/>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308" s="29" t="s">
         <v>160</v>
       </c>
@@ -7932,7 +7950,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A309" s="29"/>
       <c r="B309" s="32">
         <v>6</v>
@@ -7963,7 +7981,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A310" s="29"/>
       <c r="B310" s="32">
         <v>7</v>
@@ -7992,7 +8010,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A311" s="29"/>
       <c r="B311" s="32">
         <v>8</v>
@@ -8021,7 +8039,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A312" s="29"/>
       <c r="B312" s="32">
         <v>17</v>
@@ -8050,7 +8068,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A313" s="41"/>
       <c r="B313" s="42">
         <v>18</v>
@@ -8079,11 +8097,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D315" s="48"/>
       <c r="G315" s="46"/>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>193</v>
       </c>
@@ -8100,7 +8118,7 @@
       <c r="J316" s="32"/>
       <c r="K316" s="33"/>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B317" s="40" t="s">
         <v>51</v>
       </c>
@@ -8122,7 +8140,7 @@
       <c r="J317" s="32"/>
       <c r="K317" s="33"/>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B318" s="30" t="s">
         <v>4</v>
       </c>
@@ -8141,10 +8159,14 @@
       <c r="G318" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="J318" s="30"/>
-      <c r="K318" s="57"/>
-    </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J318" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="K318" s="57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B319">
         <v>1</v>
       </c>
@@ -8163,14 +8185,20 @@
       <c r="G319" s="13">
         <v>0.1396</v>
       </c>
-      <c r="J319" t="s">
+      <c r="J319" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K319" t="s">
+        <v>189</v>
+      </c>
+      <c r="L319" t="s">
         <v>202</v>
       </c>
-      <c r="K319" s="2" t="s">
+      <c r="M319" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B320">
         <v>2</v>
       </c>
@@ -8189,14 +8217,20 @@
       <c r="G320" s="13">
         <v>0.1396</v>
       </c>
-      <c r="J320" t="s">
+      <c r="J320" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K320" t="s">
+        <v>189</v>
+      </c>
+      <c r="L320" t="s">
         <v>165</v>
       </c>
-      <c r="K320" s="46">
+      <c r="M320" s="46">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="321" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B321">
         <v>3</v>
       </c>
@@ -8215,14 +8249,20 @@
       <c r="G321">
         <v>0.2</v>
       </c>
-      <c r="J321" t="s">
+      <c r="J321" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K321" t="s">
+        <v>189</v>
+      </c>
+      <c r="L321" t="s">
         <v>203</v>
       </c>
-      <c r="K321" s="2">
+      <c r="M321" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="322" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B322">
         <v>4</v>
       </c>
@@ -8241,9 +8281,15 @@
       <c r="G322">
         <v>0.11</v>
       </c>
-      <c r="K322" s="2"/>
-    </row>
-    <row r="323" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J322" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K322" t="s">
+        <v>189</v>
+      </c>
+      <c r="M322" s="2"/>
+    </row>
+    <row r="323" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B323">
         <v>5</v>
       </c>
@@ -8265,17 +8311,23 @@
       <c r="H323" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="J323" t="s">
+      <c r="J323" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K323" t="s">
+        <v>189</v>
+      </c>
+      <c r="L323" t="s">
         <v>2</v>
       </c>
-      <c r="K323" s="59" t="s">
+      <c r="M323" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="L323" t="s">
+      <c r="N323" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="324" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B324">
         <v>6</v>
       </c>
@@ -8291,14 +8343,20 @@
       <c r="G324">
         <v>0.13</v>
       </c>
-      <c r="K324" s="58" t="s">
+      <c r="J324" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K324" t="s">
+        <v>189</v>
+      </c>
+      <c r="M324" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="L324" t="s">
+      <c r="N324" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="325" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B325">
         <v>7</v>
       </c>
@@ -8311,14 +8369,20 @@
       <c r="E325" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K325" s="58" t="s">
+      <c r="J325" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K325" t="s">
+        <v>189</v>
+      </c>
+      <c r="M325" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="L325" t="s">
+      <c r="N325" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="326" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B326">
         <v>8</v>
       </c>
@@ -8331,14 +8395,20 @@
       <c r="E326" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="K326" s="58" t="s">
+      <c r="J326" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K326" t="s">
+        <v>189</v>
+      </c>
+      <c r="M326" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="L326" t="s">
+      <c r="N326" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="327" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B327">
         <v>9</v>
       </c>
@@ -8351,8 +8421,14 @@
       <c r="E327" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="328" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J327" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K327" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="328" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B328">
         <v>10</v>
       </c>
@@ -8365,8 +8441,14 @@
       <c r="E328" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="329" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J328" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K328" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="329" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B329">
         <v>11</v>
       </c>
@@ -8379,8 +8461,14 @@
       <c r="E329" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="330" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J329" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K329" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="330" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B330">
         <v>12</v>
       </c>
@@ -8399,8 +8487,14 @@
       <c r="G330" s="14">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="331" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J330" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K330" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="331" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B331">
         <v>13</v>
       </c>
@@ -8413,8 +8507,14 @@
       <c r="E331" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="332" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J331" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K331" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="332" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B332">
         <v>14</v>
       </c>
@@ -8427,11 +8527,14 @@
       <c r="E332" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="H332" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="333" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J332" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K332" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="333" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B333">
         <v>15</v>
       </c>
@@ -8444,11 +8547,17 @@
       <c r="E333" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="H333" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="334" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F333" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J333" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K333" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="334" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B334">
         <v>16</v>
       </c>
@@ -8461,11 +8570,17 @@
       <c r="E334" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="H334" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="335" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F334" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J334" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K334" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="335" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B335">
         <v>17</v>
       </c>
@@ -8478,8 +8593,17 @@
       <c r="E335" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="336" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F335" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J335" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K335" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="336" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B336">
         <v>18</v>
       </c>
@@ -8492,8 +8616,14 @@
       <c r="E336" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="337" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J336" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K336" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="337" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B337">
         <v>19</v>
       </c>
@@ -8506,8 +8636,14 @@
       <c r="E337" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="338" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J337" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K337" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="338" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B338">
         <v>20</v>
       </c>
@@ -8520,8 +8656,14 @@
       <c r="E338" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="339" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J338" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K338" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="339" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B339">
         <v>21</v>
       </c>
@@ -8540,8 +8682,14 @@
       <c r="G339">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="340" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J339" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K339" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="340" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B340">
         <v>22</v>
       </c>
@@ -8554,8 +8702,14 @@
       <c r="E340" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="341" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J340" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K340" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="341" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B341">
         <v>23</v>
       </c>
@@ -8568,8 +8722,14 @@
       <c r="E341" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J341" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K341" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="342" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B342">
         <v>24</v>
       </c>
@@ -8582,8 +8742,14 @@
       <c r="E342" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J342" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K342" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="343" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B343">
         <v>25</v>
       </c>
@@ -8596,8 +8762,14 @@
       <c r="E343" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J343" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K343" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="344" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B344">
         <v>26</v>
       </c>
@@ -8610,8 +8782,14 @@
       <c r="E344" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="345" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J344" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K344" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="345" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B345">
         <v>27</v>
       </c>
@@ -8624,8 +8802,14 @@
       <c r="E345" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="346" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J345" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K345" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="346" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B346">
         <v>28</v>
       </c>
@@ -8638,8 +8822,14 @@
       <c r="E346" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="347" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J346" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K346" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="347" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B347">
         <v>29</v>
       </c>
@@ -8652,8 +8842,14 @@
       <c r="E347" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="348" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J347" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K347" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="348" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B348">
         <v>30</v>
       </c>
@@ -8666,8 +8862,14 @@
       <c r="E348" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="349" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J348" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K348" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="349" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B349">
         <v>31</v>
       </c>
@@ -8683,8 +8885,14 @@
       <c r="G349">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J349" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K349" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="350" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B350">
         <v>32</v>
       </c>
@@ -8703,8 +8911,14 @@
       <c r="G350">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="351" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J350" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K350" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="351" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F351" t="s">
         <v>208</v>
       </c>
@@ -9011,7 +9225,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="369" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B369">
         <v>14</v>
       </c>
@@ -9031,7 +9245,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="370" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B370">
         <v>15</v>
       </c>
@@ -9045,7 +9259,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="371" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B371">
         <v>16</v>
       </c>
@@ -9059,7 +9273,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="372" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B372">
         <v>17</v>
       </c>
@@ -9073,7 +9287,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="373" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B373">
         <v>18</v>
       </c>
@@ -9087,7 +9301,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="374" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B374">
         <v>19</v>
       </c>
@@ -9107,7 +9321,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="375" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B375">
         <v>20</v>
       </c>
@@ -9120,11 +9334,8 @@
       <c r="E375" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="H375" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="376" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="376" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B376">
         <v>21</v>
       </c>
@@ -9137,11 +9348,11 @@
       <c r="E376" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="H376" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="377" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F376" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="377" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B377">
         <v>22</v>
       </c>
@@ -9154,11 +9365,11 @@
       <c r="E377" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="H377" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="378" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F377" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="378" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B378">
         <v>23</v>
       </c>
@@ -9171,8 +9382,11 @@
       <c r="E378" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="379" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F378" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="379" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B379">
         <v>24</v>
       </c>
@@ -9186,7 +9400,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="380" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B380">
         <v>25</v>
       </c>
@@ -9200,7 +9414,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="381" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B381">
         <v>26</v>
       </c>
@@ -9214,7 +9428,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="382" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B382">
         <v>27</v>
       </c>
@@ -9228,7 +9442,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="383" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B383">
         <v>28</v>
       </c>
@@ -9242,7 +9456,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="384" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B384">
         <v>29</v>
       </c>
@@ -9259,7 +9473,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B385">
         <v>30</v>
       </c>
@@ -9273,7 +9487,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B386">
         <v>31</v>
       </c>
@@ -9287,7 +9501,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B387">
         <v>32</v>
       </c>
@@ -9307,7 +9521,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F388" t="s">
         <v>208</v>
       </c>
@@ -9315,9 +9529,9 @@
         <v>0.13059999999999999</v>
       </c>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="B390" s="30"/>
       <c r="C390" s="30"/>
@@ -9329,7 +9543,7 @@
       <c r="G390" s="34"/>
       <c r="H390" s="38"/>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B391" s="40" t="s">
         <v>51</v>
       </c>
@@ -9348,7 +9562,7 @@
       <c r="G391" s="32"/>
       <c r="H391" s="38"/>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B392" s="30" t="s">
         <v>4</v>
       </c>
@@ -9367,8 +9581,14 @@
       <c r="G392" s="45" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J392" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="K392" s="57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B393">
         <v>1</v>
       </c>
@@ -9381,16 +9601,20 @@
       <c r="E393" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F393" s="13"/>
-      <c r="G393" s="13"/>
-      <c r="J393" t="s">
-        <v>202</v>
-      </c>
-      <c r="K393" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F393" s="13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G393" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="J393" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K393" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B394">
         <v>2</v>
       </c>
@@ -9403,14 +9627,26 @@
       <c r="E394" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="J394" t="s">
-        <v>165</v>
-      </c>
-      <c r="K394" s="46">
-        <v>5.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F394">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G394" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="J394" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K394" t="s">
+        <v>230</v>
+      </c>
+      <c r="L394" t="s">
+        <v>202</v>
+      </c>
+      <c r="M394" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B395">
         <v>3</v>
       </c>
@@ -9423,14 +9659,20 @@
       <c r="E395" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="J395" t="s">
-        <v>203</v>
-      </c>
-      <c r="K395" s="2">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J395" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K395" t="s">
+        <v>230</v>
+      </c>
+      <c r="L395" t="s">
+        <v>165</v>
+      </c>
+      <c r="M395" s="46">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B396">
         <v>4</v>
       </c>
@@ -9443,9 +9685,20 @@
       <c r="E396" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="K396" s="2"/>
-    </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J396" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K396" t="s">
+        <v>230</v>
+      </c>
+      <c r="L396" t="s">
+        <v>203</v>
+      </c>
+      <c r="M396" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B397">
         <v>5</v>
       </c>
@@ -9458,17 +9711,15 @@
       <c r="E397" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="J397" t="s">
-        <v>2</v>
+      <c r="J397" s="32" t="s">
+        <v>178</v>
       </c>
       <c r="K397" t="s">
-        <v>216</v>
-      </c>
-      <c r="L397" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="M397" s="2"/>
+    </row>
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B398">
         <v>6</v>
       </c>
@@ -9481,14 +9732,23 @@
       <c r="E398" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="J398" s="32" t="s">
+        <v>178</v>
+      </c>
       <c r="K398" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="L398" t="s">
+        <v>2</v>
+      </c>
+      <c r="M398" t="s">
+        <v>216</v>
+      </c>
+      <c r="N398" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B399">
         <v>7</v>
       </c>
@@ -9501,14 +9761,20 @@
       <c r="E399" s="13" t="s">
         <v>200</v>
       </c>
+      <c r="J399" s="32" t="s">
+        <v>179</v>
+      </c>
       <c r="K399" t="s">
-        <v>218</v>
-      </c>
-      <c r="L399" t="s">
+        <v>230</v>
+      </c>
+      <c r="M399" t="s">
+        <v>217</v>
+      </c>
+      <c r="N399" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B400">
         <v>8</v>
       </c>
@@ -9521,14 +9787,20 @@
       <c r="E400" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="J400" s="32" t="s">
+        <v>179</v>
+      </c>
       <c r="K400" t="s">
-        <v>219</v>
-      </c>
-      <c r="L400" t="s">
+        <v>230</v>
+      </c>
+      <c r="M400" t="s">
+        <v>218</v>
+      </c>
+      <c r="N400" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="401" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B401">
         <v>9</v>
       </c>
@@ -9541,8 +9813,20 @@
       <c r="E401" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="402" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J401" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K401" t="s">
+        <v>230</v>
+      </c>
+      <c r="M401" t="s">
+        <v>219</v>
+      </c>
+      <c r="N401" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="402" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B402">
         <v>10</v>
       </c>
@@ -9555,8 +9839,14 @@
       <c r="E402" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="403" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J402" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K402" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="403" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B403">
         <v>11</v>
       </c>
@@ -9569,8 +9859,20 @@
       <c r="E403" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="404" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F403">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G403" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="J403" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K403" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="404" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B404">
         <v>12</v>
       </c>
@@ -9583,8 +9885,14 @@
       <c r="E404" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="405" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J404" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K404" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="405" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B405">
         <v>13</v>
       </c>
@@ -9597,8 +9905,14 @@
       <c r="E405" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="406" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J405" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K405" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="406" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B406">
         <v>14</v>
       </c>
@@ -9611,8 +9925,14 @@
       <c r="E406" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="407" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J406" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K406" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="407" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B407">
         <v>15</v>
       </c>
@@ -9625,8 +9945,15 @@
       <c r="E407" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="408" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F407" s="2"/>
+      <c r="J407" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K407" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="408" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B408">
         <v>16</v>
       </c>
@@ -9639,8 +9966,23 @@
       <c r="E408" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="409" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F408" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G408">
+        <v>0.16</v>
+      </c>
+      <c r="H408">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J408" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K408" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="409" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B409">
         <v>17</v>
       </c>
@@ -9653,8 +9995,17 @@
       <c r="E409" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="410" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F409" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J409" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K409" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="410" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B410">
         <v>18</v>
       </c>
@@ -9667,8 +10018,17 @@
       <c r="E410" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="411" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F410" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J410" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="K410" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="411" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B411">
         <v>19</v>
       </c>
@@ -9681,8 +10041,14 @@
       <c r="E411" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="412" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J411" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K411" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="412" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B412">
         <v>20</v>
       </c>
@@ -9695,8 +10061,14 @@
       <c r="E412" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="413" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J412" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K412" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="413" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B413">
         <v>21</v>
       </c>
@@ -9709,8 +10081,20 @@
       <c r="E413" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="414" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F413">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G413">
+        <v>0.08</v>
+      </c>
+      <c r="J413" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K413" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="414" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B414">
         <v>22</v>
       </c>
@@ -9723,8 +10107,20 @@
       <c r="E414" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="415" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F414">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G414">
+        <v>0.05</v>
+      </c>
+      <c r="J414" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K414" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="415" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B415">
         <v>23</v>
       </c>
@@ -9737,8 +10133,14 @@
       <c r="E415" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="416" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J415" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K415" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="416" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B416">
         <v>24</v>
       </c>
@@ -9751,8 +10153,14 @@
       <c r="E416" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="417" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J416" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="K416" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="417" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B417">
         <v>25</v>
       </c>
@@ -9765,8 +10173,14 @@
       <c r="E417" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="418" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J417" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K417" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="418" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B418">
         <v>26</v>
       </c>
@@ -9779,8 +10193,14 @@
       <c r="E418" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="419" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J418" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="K418" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="419" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B419">
         <v>27</v>
       </c>
@@ -9793,8 +10213,14 @@
       <c r="E419" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="420" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J419" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K419" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="420" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B420">
         <v>28</v>
       </c>
@@ -9807,8 +10233,14 @@
       <c r="E420" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="421" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J420" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="K420" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="421" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B421">
         <v>29</v>
       </c>
@@ -9821,8 +10253,14 @@
       <c r="E421" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="422" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J421" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K421" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="422" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B422">
         <v>30</v>
       </c>
@@ -9835,8 +10273,14 @@
       <c r="E422" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="423" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J422" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K422" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="423" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B423">
         <v>31</v>
       </c>
@@ -9849,8 +10293,14 @@
       <c r="E423" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="424" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J423" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K423" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="424" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B424">
         <v>32</v>
       </c>
@@ -9862,6 +10312,26 @@
       </c>
       <c r="E424" s="14" t="s">
         <v>201</v>
+      </c>
+      <c r="F424">
+        <v>0.05</v>
+      </c>
+      <c r="G424">
+        <v>0.06</v>
+      </c>
+      <c r="J424" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="K424" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="425" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F425" t="s">
+        <v>227</v>
+      </c>
+      <c r="G425">
+        <v>8.0560000000000007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results and pictures batch 60 and 80sect
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12720" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="237">
   <si>
     <t>Alfa</t>
   </si>
@@ -712,6 +713,21 @@
   </si>
   <si>
     <t>magenta</t>
+  </si>
+  <si>
+    <t>SOA_formation_05072013_batch_10nm_60sect</t>
+  </si>
+  <si>
+    <t>SOA_formation_05072013_batch_80_isoM_60sect</t>
+  </si>
+  <si>
+    <t>vastaava kuin yllä mutta enemmän sektioita ja Dp yläraja 1e-5 -&gt; 1e-6</t>
+  </si>
+  <si>
+    <t>run_20130710T200107</t>
+  </si>
+  <si>
+    <t>run_20130710T205749</t>
   </si>
 </sst>
 </file>
@@ -1345,10 +1361,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N425"/>
+  <dimension ref="A1:N433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H339" sqref="H339"/>
+    <sheetView tabSelected="1" topLeftCell="A417" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B435" sqref="B435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,7 +1574,7 @@
         <v>1000</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8" si="1">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F8">
@@ -1616,7 +1632,7 @@
         <v>1000</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10" si="2">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F10">
@@ -1665,7 +1681,7 @@
         <v>1000</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12" si="3">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F12">
@@ -1737,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15:H23" si="4">F15*0.00000000000000009*0.00000003*26908000000000000000*G15*0.000000001*26908000000000000000</f>
+        <f t="shared" ref="H15:H23" si="1">F15*0.00000000000000009*0.00000003*26908000000000000000*G15*0.000000001*26908000000000000000</f>
         <v>586472.77584000002</v>
       </c>
       <c r="J15" t="s">
@@ -1767,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1172945.55168</v>
       </c>
     </row>
@@ -1795,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1172945.55168</v>
       </c>
       <c r="J17" t="s">
@@ -1825,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1759418.3275199998</v>
       </c>
     </row>
@@ -1843,7 +1859,7 @@
         <v>2000</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19" si="5">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F19">
@@ -1853,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1759418.3275199998</v>
       </c>
       <c r="J19" t="s">
@@ -1883,7 +1899,7 @@
         <v>0.25</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>146618.19396</v>
       </c>
     </row>
@@ -1901,7 +1917,7 @@
         <v>2000</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21" si="6">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F21">
@@ -1911,7 +1927,7 @@
         <v>0.25</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>146618.19396</v>
       </c>
     </row>
@@ -1935,7 +1951,7 @@
         <v>1.5</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>879709.16375999991</v>
       </c>
     </row>
@@ -1950,7 +1966,7 @@
         <v>2000</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23" si="7">$E$4</f>
+        <f>$E$4</f>
         <v>0</v>
       </c>
       <c r="F23">
@@ -1960,7 +1976,7 @@
         <v>1.5</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>879709.16375999991</v>
       </c>
     </row>
@@ -1995,7 +2011,7 @@
         <v>100</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" ref="H25:H30" si="8">F25*0.0000000000000002*0.00000006*26908000000000000000*G25*0.000000001*26908000000000000000</f>
+        <f t="shared" ref="H25:H30" si="2">F25*0.0000000000000002*0.00000006*26908000000000000000*G25*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I25" t="s">
@@ -2028,7 +2044,7 @@
         <v>100</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>260654567.04000002</v>
       </c>
       <c r="L26" t="s">
@@ -2058,7 +2074,7 @@
         <v>100</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>521309134.08000004</v>
       </c>
       <c r="I27" t="s">
@@ -2091,7 +2107,7 @@
         <v>100</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>521309134.08000004</v>
       </c>
     </row>
@@ -2118,7 +2134,7 @@
         <v>100</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>781963701.12</v>
       </c>
       <c r="J29" t="s">
@@ -2151,7 +2167,7 @@
         <v>100</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>781963701.12</v>
       </c>
       <c r="K30" t="s">
@@ -2192,7 +2208,7 @@
         <v>100</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" ref="H33:H38" si="9">F33*0.0000000000000002*0.00000006*26908000000000000000*G33*0.000000001*26908000000000000000</f>
+        <f t="shared" ref="H33:H38" si="3">F33*0.0000000000000002*0.00000006*26908000000000000000*G33*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I33" t="s">
@@ -2225,7 +2241,7 @@
         <v>100</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>260654567.04000002</v>
       </c>
       <c r="I34" t="s">
@@ -2258,7 +2274,7 @@
         <v>100</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>521309134.08000004</v>
       </c>
       <c r="J35" t="s">
@@ -2288,7 +2304,7 @@
         <v>100</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>521309134.08000004</v>
       </c>
       <c r="I36" t="s">
@@ -2318,7 +2334,7 @@
         <v>100</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>781963701.12</v>
       </c>
       <c r="J37" s="1" t="s">
@@ -2348,7 +2364,7 @@
         <v>100</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>781963701.12</v>
       </c>
       <c r="J38" s="1" t="s">
@@ -2395,7 +2411,7 @@
         <v>100</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" ref="H41" si="10">F41*0.0000000000000002*0.00000006*26908000000000000000*G41*0.000000001*26908000000000000000</f>
+        <f>F41*0.0000000000000002*0.00000006*26908000000000000000*G41*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I41" s="10" t="s">
@@ -2466,7 +2482,7 @@
         <v>100</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" ref="H47" si="11">F47*0.0000000000000002*0.00000006*26908000000000000000*G47*0.000000001*26908000000000000000</f>
+        <f>F47*0.0000000000000002*0.00000006*26908000000000000000*G47*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I47" s="10" t="s">
@@ -2502,7 +2518,7 @@
         <v>100</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" ref="H48" si="12">F48*0.0000000000000002*0.00000006*26908000000000000000*G48*0.000000001*26908000000000000000</f>
+        <f>F48*0.0000000000000002*0.00000006*26908000000000000000*G48*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I48" s="10" t="s">
@@ -2911,7 +2927,7 @@
         <v>100</v>
       </c>
       <c r="H75" s="2">
-        <f t="shared" ref="H75" si="13">F75*0.0000000000000002*0.00000006*26908000000000000000*G75*0.000000001*26908000000000000000</f>
+        <f>F75*0.0000000000000002*0.00000006*26908000000000000000*G75*0.000000001*26908000000000000000</f>
         <v>260654567.04000002</v>
       </c>
       <c r="I75" s="10" t="s">
@@ -10160,7 +10176,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="417" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B417">
         <v>25</v>
       </c>
@@ -10180,7 +10196,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="418" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B418">
         <v>26</v>
       </c>
@@ -10200,7 +10216,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="419" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B419">
         <v>27</v>
       </c>
@@ -10220,7 +10236,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="420" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B420">
         <v>28</v>
       </c>
@@ -10240,7 +10256,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="421" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B421">
         <v>29</v>
       </c>
@@ -10260,7 +10276,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="422" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B422">
         <v>30</v>
       </c>
@@ -10280,7 +10296,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="423" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B423">
         <v>31</v>
       </c>
@@ -10300,7 +10316,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="424" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B424">
         <v>32</v>
       </c>
@@ -10326,12 +10342,66 @@
         <v>231</v>
       </c>
     </row>
-    <row r="425" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F425" t="s">
         <v>227</v>
       </c>
       <c r="G425">
         <v>8.0560000000000007E-2</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>232</v>
+      </c>
+      <c r="B428" s="30"/>
+      <c r="C428" s="30"/>
+      <c r="D428" s="30"/>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>236</v>
+      </c>
+      <c r="B429" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C430" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>233</v>
+      </c>
+      <c r="B431" s="30"/>
+      <c r="C431" s="30"/>
+      <c r="D431" s="30"/>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>235</v>
+      </c>
+      <c r="B432" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="433" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C433" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final CS and Moa figs, matlab2tikz, linewidth
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1363,8 +1362,8 @@
   </sheetPr>
   <dimension ref="A1:N433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B435" sqref="B435"/>
+    <sheetView tabSelected="1" topLeftCell="A390" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C403" sqref="C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9545,6 +9544,12 @@
         <v>0.13059999999999999</v>
       </c>
     </row>
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G389">
+        <f>24*G388</f>
+        <v>3.1343999999999999</v>
+      </c>
+    </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>228</v>
@@ -10348,6 +10353,12 @@
       </c>
       <c r="G425">
         <v>8.0560000000000007E-2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G426">
+        <f>24*G425</f>
+        <v>1.93344</v>
       </c>
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Batch, fixed Diff and Molemass, results and figs
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="242">
   <si>
     <t>Alfa</t>
   </si>
@@ -727,6 +727,21 @@
   </si>
   <si>
     <t>run_20130710T205749</t>
+  </si>
+  <si>
+    <t>run_20130722T205812</t>
+  </si>
+  <si>
+    <t>run_20130722T202717</t>
+  </si>
+  <si>
+    <t>SOA_formation_22072013_batch_10nm_60sect</t>
+  </si>
+  <si>
+    <t>SOA_formation_22072013_batch_80_isoM_60sect</t>
+  </si>
+  <si>
+    <t>vastaava kuin yllä mutta muutettu diffuusiokerroin,vapaamatka,tiheys ja moolimassa</t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1375,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N433"/>
+  <dimension ref="A1:N441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C403" sqref="C403"/>
+    <sheetView tabSelected="1" topLeftCell="A426" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C441" sqref="C441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10410,9 +10425,63 @@
         <v>199</v>
       </c>
     </row>
-    <row r="433" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C433" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>239</v>
+      </c>
+      <c r="B436" s="30"/>
+      <c r="C436" s="30"/>
+      <c r="D436" s="30"/>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>237</v>
+      </c>
+      <c r="B437" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C438" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>240</v>
+      </c>
+      <c r="B439" s="30"/>
+      <c r="C439" s="30"/>
+      <c r="D439" s="30"/>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>238</v>
+      </c>
+      <c r="B440" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C441" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited Vtot to be drawn as batch
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="247">
   <si>
     <t>Alfa</t>
   </si>
@@ -742,6 +742,21 @@
   </si>
   <si>
     <t>vastaava kuin yllä mutta muutettu diffuusiokerroin,vapaamatka,tiheys ja moolimassa</t>
+  </si>
+  <si>
+    <t>SOA_formation_23072013_batch_80_isoM_60sect</t>
+  </si>
+  <si>
+    <t>SOA_formation_23072013_batch_10nm_60sect</t>
+  </si>
+  <si>
+    <t>vastaava kuin yllä mutta muutettu vapaamatka 300 -&gt;100</t>
+  </si>
+  <si>
+    <t>run_20130723T161001</t>
+  </si>
+  <si>
+    <t>run_20130723T154011</t>
   </si>
 </sst>
 </file>
@@ -1375,10 +1390,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N441"/>
+  <dimension ref="A1:N448"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A426" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C441" sqref="C441"/>
+      <selection activeCell="C451" sqref="C451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10482,6 +10497,60 @@
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C441" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>243</v>
+      </c>
+      <c r="B443" s="30"/>
+      <c r="C443" s="30"/>
+      <c r="D443" s="30"/>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>245</v>
+      </c>
+      <c r="B444" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C445" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>242</v>
+      </c>
+      <c r="B446" s="30"/>
+      <c r="C446" s="30"/>
+      <c r="D446" s="30"/>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>246</v>
+      </c>
+      <c r="B447" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D447" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C448" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed correct density to, results
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/SOA formation/Runs.xlsx
+++ b/Results and scripts_mp/SOA formation/Runs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="249">
   <si>
     <t>Alfa</t>
   </si>
@@ -757,6 +757,12 @@
   </si>
   <si>
     <t>run_20130723T154011</t>
+  </si>
+  <si>
+    <t>Lisäksi vielä tiheydet 1.84 -&gt;1.4 funktiossa mass2number</t>
+  </si>
+  <si>
+    <t>Vtot plot mark</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,6 +823,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1013,7 +1025,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1076,6 +1088,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent2" xfId="10" builtinId="34"/>
@@ -1092,6 +1105,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC00CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1390,10 +1408,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N448"/>
+  <dimension ref="A1:P451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C451" sqref="C451"/>
+    <sheetView tabSelected="1" topLeftCell="B382" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J388" sqref="J388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7907,7 +7925,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A305" s="29"/>
       <c r="B305" s="32"/>
       <c r="C305" s="32"/>
@@ -7920,7 +7938,7 @@
       <c r="J305" s="32"/>
       <c r="K305" s="33"/>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A306" s="29"/>
       <c r="B306" s="32"/>
       <c r="C306" s="32"/>
@@ -7935,7 +7953,7 @@
       <c r="J306" s="32"/>
       <c r="K306" s="33"/>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A307" s="53" t="s">
         <v>139</v>
       </c>
@@ -7962,7 +7980,7 @@
       <c r="J307" s="32"/>
       <c r="K307" s="33"/>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A308" s="29" t="s">
         <v>160</v>
       </c>
@@ -7995,7 +8013,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A309" s="29"/>
       <c r="B309" s="32">
         <v>6</v>
@@ -8026,7 +8044,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A310" s="29"/>
       <c r="B310" s="32">
         <v>7</v>
@@ -8055,7 +8073,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A311" s="29"/>
       <c r="B311" s="32">
         <v>8</v>
@@ -8084,7 +8102,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A312" s="29"/>
       <c r="B312" s="32">
         <v>17</v>
@@ -8113,7 +8131,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A313" s="41"/>
       <c r="B313" s="42">
         <v>18</v>
@@ -8142,11 +8160,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D315" s="48"/>
       <c r="G315" s="46"/>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>193</v>
       </c>
@@ -8163,7 +8181,7 @@
       <c r="J316" s="32"/>
       <c r="K316" s="33"/>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B317" s="40" t="s">
         <v>51</v>
       </c>
@@ -8185,7 +8203,7 @@
       <c r="J317" s="32"/>
       <c r="K317" s="33"/>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B318" s="30" t="s">
         <v>4</v>
       </c>
@@ -8210,8 +8228,14 @@
       <c r="K318" s="57" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L318" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="M318" s="45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B319">
         <v>1</v>
       </c>
@@ -8233,17 +8257,23 @@
       <c r="J319" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K319" t="s">
+      <c r="K319" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="L319" t="s">
+      <c r="L319" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M319" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="N319" t="s">
         <v>202</v>
       </c>
-      <c r="M319" s="2" t="s">
+      <c r="O319" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B320">
         <v>2</v>
       </c>
@@ -8265,17 +8295,23 @@
       <c r="J320" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K320" t="s">
+      <c r="K320" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="L320" t="s">
+      <c r="L320" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M320" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="N320" t="s">
         <v>165</v>
       </c>
-      <c r="M320" s="46">
+      <c r="O320" s="46">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="321" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B321">
         <v>3</v>
       </c>
@@ -8297,17 +8333,23 @@
       <c r="J321" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K321" t="s">
+      <c r="K321" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="L321" t="s">
+      <c r="L321" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M321" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="N321" t="s">
         <v>203</v>
       </c>
-      <c r="M321" s="2">
+      <c r="O321" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="322" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B322">
         <v>4</v>
       </c>
@@ -8329,12 +8371,18 @@
       <c r="J322" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K322" t="s">
+      <c r="K322" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="M322" s="2"/>
-    </row>
-    <row r="323" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L322" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M322" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="O322" s="2"/>
+    </row>
+    <row r="323" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B323">
         <v>5</v>
       </c>
@@ -8359,20 +8407,26 @@
       <c r="J323" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K323" t="s">
+      <c r="K323" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="L323" t="s">
+      <c r="L323" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M323" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="N323" t="s">
         <v>2</v>
       </c>
-      <c r="M323" s="59" t="s">
+      <c r="O323" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="N323" t="s">
+      <c r="P323" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="324" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B324">
         <v>6</v>
       </c>
@@ -8391,17 +8445,23 @@
       <c r="J324" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K324" t="s">
+      <c r="K324" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="M324" s="58" t="s">
+      <c r="L324" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M324" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="O324" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="N324" t="s">
+      <c r="P324" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="325" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B325">
         <v>7</v>
       </c>
@@ -8417,17 +8477,23 @@
       <c r="J325" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K325" t="s">
+      <c r="K325" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="M325" s="58" t="s">
+      <c r="L325" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M325" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="O325" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="N325" t="s">
+      <c r="P325" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="326" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B326">
         <v>8</v>
       </c>
@@ -8443,17 +8509,23 @@
       <c r="J326" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K326" t="s">
+      <c r="K326" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="M326" s="58" t="s">
+      <c r="L326" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M326" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="O326" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="N326" t="s">
+      <c r="P326" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="327" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B327">
         <v>9</v>
       </c>
@@ -8469,11 +8541,17 @@
       <c r="J327" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K327" t="s">
+      <c r="K327" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="328" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L327" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M327" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="328" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B328">
         <v>10</v>
       </c>
@@ -8489,11 +8567,17 @@
       <c r="J328" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K328" t="s">
+      <c r="K328" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="329" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L328" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M328" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="329" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B329">
         <v>11</v>
       </c>
@@ -8509,11 +8593,17 @@
       <c r="J329" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K329" t="s">
+      <c r="K329" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="330" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L329" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M329" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="330" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B330">
         <v>12</v>
       </c>
@@ -8535,11 +8625,17 @@
       <c r="J330" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K330" t="s">
+      <c r="K330" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="331" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L330" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M330" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="331" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B331">
         <v>13</v>
       </c>
@@ -8555,11 +8651,17 @@
       <c r="J331" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K331" t="s">
+      <c r="K331" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="332" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L331" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M331" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="332" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B332">
         <v>14</v>
       </c>
@@ -8575,11 +8677,17 @@
       <c r="J332" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K332" t="s">
+      <c r="K332" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="333" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L332" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M332" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="333" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B333">
         <v>15</v>
       </c>
@@ -8598,11 +8706,17 @@
       <c r="J333" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K333" t="s">
+      <c r="K333" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="334" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L333" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M333" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="334" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B334">
         <v>16</v>
       </c>
@@ -8621,11 +8735,17 @@
       <c r="J334" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K334" t="s">
+      <c r="K334" s="60" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="335" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L334" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M334" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="335" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B335">
         <v>17</v>
       </c>
@@ -8647,8 +8767,14 @@
       <c r="K335" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="336" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L335" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M335" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="336" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B336">
         <v>18</v>
       </c>
@@ -8667,8 +8793,14 @@
       <c r="K336" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="337" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L336" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M336" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="337" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B337">
         <v>19</v>
       </c>
@@ -8687,8 +8819,14 @@
       <c r="K337" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="338" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L337" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M337" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="338" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B338">
         <v>20</v>
       </c>
@@ -8707,8 +8845,14 @@
       <c r="K338" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="339" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L338" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M338" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="339" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B339">
         <v>21</v>
       </c>
@@ -8733,8 +8877,14 @@
       <c r="K339" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="340" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L339" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M339" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="340" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B340">
         <v>22</v>
       </c>
@@ -8753,8 +8903,14 @@
       <c r="K340" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="341" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L340" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M340" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="341" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B341">
         <v>23</v>
       </c>
@@ -8773,8 +8929,14 @@
       <c r="K341" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="342" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L341" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M341" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="342" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B342">
         <v>24</v>
       </c>
@@ -8793,8 +8955,14 @@
       <c r="K342" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="343" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L342" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M342" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="343" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B343">
         <v>25</v>
       </c>
@@ -8813,8 +8981,14 @@
       <c r="K343" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="344" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L343" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M343" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="344" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B344">
         <v>26</v>
       </c>
@@ -8833,8 +9007,14 @@
       <c r="K344" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="345" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L344" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M344" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="345" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B345">
         <v>27</v>
       </c>
@@ -8853,8 +9033,14 @@
       <c r="K345" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="346" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L345" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M345" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="346" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B346">
         <v>28</v>
       </c>
@@ -8873,8 +9059,14 @@
       <c r="K346" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="347" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L346" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M346" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="347" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B347">
         <v>29</v>
       </c>
@@ -8893,8 +9085,14 @@
       <c r="K347" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="348" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L347" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M347" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="348" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B348">
         <v>30</v>
       </c>
@@ -8913,8 +9111,14 @@
       <c r="K348" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="349" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L348" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M348" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="349" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B349">
         <v>31</v>
       </c>
@@ -8936,8 +9140,14 @@
       <c r="K349" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="350" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L349" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M349" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="350" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B350">
         <v>32</v>
       </c>
@@ -8962,8 +9172,14 @@
       <c r="K350" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="351" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L350" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M350" s="60" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="351" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F351" t="s">
         <v>208</v>
       </c>
@@ -9518,7 +9734,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B385">
         <v>30</v>
       </c>
@@ -9532,7 +9748,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B386">
         <v>31</v>
       </c>
@@ -9546,7 +9762,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B387">
         <v>32</v>
       </c>
@@ -9566,7 +9782,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F388" t="s">
         <v>208</v>
       </c>
@@ -9574,13 +9790,13 @@
         <v>0.13059999999999999</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G389">
         <f>24*G388</f>
         <v>3.1343999999999999</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>228</v>
       </c>
@@ -9594,7 +9810,7 @@
       <c r="G390" s="34"/>
       <c r="H390" s="38"/>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B391" s="40" t="s">
         <v>51</v>
       </c>
@@ -9613,7 +9829,7 @@
       <c r="G391" s="32"/>
       <c r="H391" s="38"/>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B392" s="30" t="s">
         <v>4</v>
       </c>
@@ -9638,8 +9854,14 @@
       <c r="K392" s="57" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L392" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="M392" s="45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="393" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B393">
         <v>1</v>
       </c>
@@ -9661,11 +9883,17 @@
       <c r="J393" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K393" t="s">
+      <c r="K393" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L393" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M393" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="394" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B394">
         <v>2</v>
       </c>
@@ -9687,17 +9915,23 @@
       <c r="J394" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K394" t="s">
+      <c r="K394" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="L394" t="s">
+      <c r="L394" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M394" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="N394" t="s">
         <v>202</v>
       </c>
-      <c r="M394" s="2" t="s">
+      <c r="O394" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B395">
         <v>3</v>
       </c>
@@ -9713,17 +9947,23 @@
       <c r="J395" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K395" t="s">
+      <c r="K395" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="L395" t="s">
+      <c r="L395" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M395" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="N395" t="s">
         <v>165</v>
       </c>
-      <c r="M395" s="46">
+      <c r="O395" s="46">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B396">
         <v>4</v>
       </c>
@@ -9739,17 +9979,23 @@
       <c r="J396" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K396" t="s">
+      <c r="K396" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="L396" t="s">
+      <c r="L396" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M396" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="N396" t="s">
         <v>203</v>
       </c>
-      <c r="M396" s="2">
+      <c r="O396" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B397">
         <v>5</v>
       </c>
@@ -9765,12 +10011,18 @@
       <c r="J397" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K397" t="s">
+      <c r="K397" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="M397" s="2"/>
-    </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L397" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M397" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="O397" s="2"/>
+    </row>
+    <row r="398" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B398">
         <v>6</v>
       </c>
@@ -9786,20 +10038,26 @@
       <c r="J398" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K398" t="s">
+      <c r="K398" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="L398" t="s">
+      <c r="L398" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M398" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="N398" t="s">
         <v>2</v>
       </c>
-      <c r="M398" t="s">
+      <c r="O398" t="s">
         <v>216</v>
       </c>
-      <c r="N398" t="s">
+      <c r="P398" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B399">
         <v>7</v>
       </c>
@@ -9815,17 +10073,23 @@
       <c r="J399" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K399" t="s">
+      <c r="K399" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="M399" t="s">
+      <c r="L399" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M399" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="O399" t="s">
         <v>217</v>
       </c>
-      <c r="N399" t="s">
+      <c r="P399" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B400">
         <v>8</v>
       </c>
@@ -9841,17 +10105,23 @@
       <c r="J400" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K400" t="s">
+      <c r="K400" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="M400" t="s">
+      <c r="L400" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M400" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="O400" t="s">
         <v>218</v>
       </c>
-      <c r="N400" t="s">
+      <c r="P400" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="401" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B401">
         <v>9</v>
       </c>
@@ -9867,17 +10137,23 @@
       <c r="J401" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K401" t="s">
+      <c r="K401" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="M401" t="s">
+      <c r="L401" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M401" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="O401" t="s">
         <v>219</v>
       </c>
-      <c r="N401" t="s">
+      <c r="P401" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="402" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B402">
         <v>10</v>
       </c>
@@ -9893,11 +10169,17 @@
       <c r="J402" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K402" t="s">
+      <c r="K402" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="403" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L402" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M402" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="403" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B403">
         <v>11</v>
       </c>
@@ -9919,11 +10201,17 @@
       <c r="J403" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K403" t="s">
+      <c r="K403" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="404" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L403" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M403" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="404" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B404">
         <v>12</v>
       </c>
@@ -9939,11 +10227,17 @@
       <c r="J404" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K404" t="s">
+      <c r="K404" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="405" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L404" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M404" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="405" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B405">
         <v>13</v>
       </c>
@@ -9959,11 +10253,17 @@
       <c r="J405" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K405" t="s">
+      <c r="K405" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="406" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L405" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M405" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="406" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B406">
         <v>14</v>
       </c>
@@ -9979,11 +10279,17 @@
       <c r="J406" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K406" t="s">
+      <c r="K406" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="407" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L406" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M406" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="407" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B407">
         <v>15</v>
       </c>
@@ -10000,11 +10306,17 @@
       <c r="J407" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K407" t="s">
+      <c r="K407" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="408" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L407" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="M407" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="408" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B408">
         <v>16</v>
       </c>
@@ -10029,11 +10341,17 @@
       <c r="J408" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K408" t="s">
+      <c r="K408" s="60" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="409" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L408" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="M408" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="409" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B409">
         <v>17</v>
       </c>
@@ -10052,11 +10370,17 @@
       <c r="J409" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K409" t="s">
+      <c r="K409" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="410" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L409" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M409" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="410" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B410">
         <v>18</v>
       </c>
@@ -10075,11 +10399,17 @@
       <c r="J410" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="K410" t="s">
+      <c r="K410" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="411" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L410" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M410" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="411" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B411">
         <v>19</v>
       </c>
@@ -10095,11 +10425,17 @@
       <c r="J411" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K411" t="s">
+      <c r="K411" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="412" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L411" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M411" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="412" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B412">
         <v>20</v>
       </c>
@@ -10115,11 +10451,17 @@
       <c r="J412" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="K412" t="s">
+      <c r="K412" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="413" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L412" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M412" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="413" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B413">
         <v>21</v>
       </c>
@@ -10141,11 +10483,17 @@
       <c r="J413" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K413" t="s">
+      <c r="K413" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="414" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L413" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M413" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="414" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B414">
         <v>22</v>
       </c>
@@ -10167,11 +10515,17 @@
       <c r="J414" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="K414" t="s">
+      <c r="K414" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="415" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L414" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M414" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="415" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B415">
         <v>23</v>
       </c>
@@ -10187,11 +10541,17 @@
       <c r="J415" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K415" t="s">
+      <c r="K415" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="416" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L415" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="M415" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="416" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B416">
         <v>24</v>
       </c>
@@ -10207,11 +10567,17 @@
       <c r="J416" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="K416" t="s">
+      <c r="K416" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L416" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="M416" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B417">
         <v>25</v>
       </c>
@@ -10227,11 +10593,17 @@
       <c r="J417" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K417" t="s">
+      <c r="K417" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L417" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M417" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B418">
         <v>26</v>
       </c>
@@ -10247,11 +10619,17 @@
       <c r="J418" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="K418" t="s">
+      <c r="K418" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L418" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M418" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B419">
         <v>27</v>
       </c>
@@ -10267,11 +10645,17 @@
       <c r="J419" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K419" t="s">
+      <c r="K419" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L419" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M419" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="420" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B420">
         <v>28</v>
       </c>
@@ -10287,11 +10671,17 @@
       <c r="J420" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="K420" t="s">
+      <c r="K420" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L420" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M420" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B421">
         <v>29</v>
       </c>
@@ -10307,11 +10697,17 @@
       <c r="J421" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K421" t="s">
+      <c r="K421" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L421" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M421" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="422" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B422">
         <v>30</v>
       </c>
@@ -10327,11 +10723,17 @@
       <c r="J422" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K422" t="s">
+      <c r="K422" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L422" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M422" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B423">
         <v>31</v>
       </c>
@@ -10347,11 +10749,17 @@
       <c r="J423" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K423" t="s">
+      <c r="K423" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L423" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="M423" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="424" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B424">
         <v>32</v>
       </c>
@@ -10373,11 +10781,17 @@
       <c r="J424" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K424" t="s">
+      <c r="K424" s="60" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L424" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M424" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F425" t="s">
         <v>227</v>
       </c>
@@ -10385,13 +10799,13 @@
         <v>8.0560000000000007E-2</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G426">
         <f>24*G425</f>
         <v>1.93344</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>232</v>
       </c>
@@ -10399,7 +10813,7 @@
       <c r="C428" s="30"/>
       <c r="D428" s="30"/>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>236</v>
       </c>
@@ -10413,12 +10827,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C430" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>233</v>
       </c>
@@ -10426,7 +10840,7 @@
       <c r="C431" s="30"/>
       <c r="D431" s="30"/>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>235</v>
       </c>
@@ -10551,6 +10965,11 @@
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C448" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="451" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C451" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>